<commit_message>
updated message for mask
</commit_message>
<xml_diff>
--- a/blinka/data/grid.xlsx
+++ b/blinka/data/grid.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\william.harding\Documents\repos\raspberrypi\blinka\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\source\repos\raspberrypi\blinka\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA40D897-CBB9-4B7D-BC37-7B03D1087789}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDB4828-517B-4DB1-B378-D0C98A995A6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5130" yWindow="3060" windowWidth="43560" windowHeight="19155" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mask" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,9 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>IN</t>
   </si>
 </sst>
 </file>
@@ -368,16 +372,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,26 +404,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -429,7 +433,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -437,7 +441,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -446,7 +450,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -455,17 +459,17 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -474,4 +478,355 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7823F826-DB8C-4CD7-AE29-877D52C9DD1E}">
+  <dimension ref="C3:M19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O27" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="4" customWidth="1"/>
+    <col min="5" max="12" width="4.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>29</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>28</v>
+      </c>
+      <c r="G5">
+        <v>31</v>
+      </c>
+      <c r="H5">
+        <v>42</v>
+      </c>
+      <c r="I5">
+        <v>44</v>
+      </c>
+      <c r="J5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>27</v>
+      </c>
+      <c r="G6">
+        <v>32</v>
+      </c>
+      <c r="H6">
+        <v>41</v>
+      </c>
+      <c r="I6">
+        <v>45</v>
+      </c>
+      <c r="J6">
+        <v>54</v>
+      </c>
+      <c r="K6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>26</v>
+      </c>
+      <c r="G7">
+        <v>33</v>
+      </c>
+      <c r="H7">
+        <v>40</v>
+      </c>
+      <c r="I7">
+        <v>46</v>
+      </c>
+      <c r="J7">
+        <v>53</v>
+      </c>
+      <c r="K7">
+        <v>57</v>
+      </c>
+      <c r="L7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>34</v>
+      </c>
+      <c r="H8">
+        <v>39</v>
+      </c>
+      <c r="I8">
+        <v>47</v>
+      </c>
+      <c r="J8">
+        <v>52</v>
+      </c>
+      <c r="K8">
+        <v>58</v>
+      </c>
+      <c r="L8">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <v>35</v>
+      </c>
+      <c r="H9">
+        <v>38</v>
+      </c>
+      <c r="I9">
+        <v>48</v>
+      </c>
+      <c r="J9">
+        <v>51</v>
+      </c>
+      <c r="K9">
+        <v>59</v>
+      </c>
+      <c r="L9">
+        <v>62</v>
+      </c>
+      <c r="M9">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>23</v>
+      </c>
+      <c r="G10">
+        <v>36</v>
+      </c>
+      <c r="H10">
+        <v>37</v>
+      </c>
+      <c r="I10">
+        <v>49</v>
+      </c>
+      <c r="J10">
+        <v>50</v>
+      </c>
+      <c r="K10">
+        <v>60</v>
+      </c>
+      <c r="L10">
+        <v>61</v>
+      </c>
+      <c r="M10">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>98</v>
+      </c>
+      <c r="E12">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>22</v>
+      </c>
+      <c r="H12">
+        <v>97</v>
+      </c>
+      <c r="I12">
+        <v>87</v>
+      </c>
+      <c r="J12">
+        <v>86</v>
+      </c>
+      <c r="K12">
+        <v>77</v>
+      </c>
+      <c r="L12">
+        <v>76</v>
+      </c>
+      <c r="M12">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>21</v>
+      </c>
+      <c r="H13">
+        <v>96</v>
+      </c>
+      <c r="I13">
+        <v>88</v>
+      </c>
+      <c r="J13">
+        <v>85</v>
+      </c>
+      <c r="K13">
+        <v>78</v>
+      </c>
+      <c r="L13">
+        <v>75</v>
+      </c>
+      <c r="M13">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="H14">
+        <v>95</v>
+      </c>
+      <c r="I14">
+        <v>89</v>
+      </c>
+      <c r="J14">
+        <v>84</v>
+      </c>
+      <c r="K14">
+        <v>79</v>
+      </c>
+      <c r="L14">
+        <v>74</v>
+      </c>
+      <c r="M14">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>19</v>
+      </c>
+      <c r="H15">
+        <v>94</v>
+      </c>
+      <c r="I15">
+        <v>90</v>
+      </c>
+      <c r="J15">
+        <v>83</v>
+      </c>
+      <c r="K15">
+        <v>80</v>
+      </c>
+      <c r="L15">
+        <v>73</v>
+      </c>
+      <c r="M15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>11</v>
+      </c>
+      <c r="F16">
+        <v>18</v>
+      </c>
+      <c r="H16">
+        <v>93</v>
+      </c>
+      <c r="I16">
+        <v>91</v>
+      </c>
+      <c r="J16">
+        <v>82</v>
+      </c>
+      <c r="K16">
+        <v>81</v>
+      </c>
+      <c r="L16">
+        <v>72</v>
+      </c>
+      <c r="M16">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>17</v>
+      </c>
+      <c r="H17">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>13</v>
+      </c>
+      <c r="F18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>14</v>
+      </c>
+      <c r="F19">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated excel reading format
</commit_message>
<xml_diff>
--- a/blinka/data/grid.xlsx
+++ b/blinka/data/grid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\william.harding\Documents\repos\raspberrypi\blinka\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1729CA73-60B6-4F45-B1DE-7882E2B8216A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC9CF45-FB66-40B2-B5AF-0E46E8D64B1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="setup" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="4">
   <si>
     <t>IN</t>
   </si>
@@ -49,7 +49,7 @@
     <t/>
   </si>
   <si>
-    <t>(100,100,100)</t>
+    <t>100,100,100</t>
   </si>
 </sst>
 </file>
@@ -370,7 +370,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -394,8 +394,8 @@
         <v>100</v>
       </c>
       <c r="F1" t="str">
-        <f>"("&amp;B1&amp;","&amp;C1&amp;","&amp;D1&amp;")"</f>
-        <v>(100,100,100)</v>
+        <f>B1&amp;","&amp;C1&amp;","&amp;D1</f>
+        <v>100,100,100</v>
       </c>
     </row>
   </sheetData>
@@ -409,7 +409,7 @@
   <dimension ref="C3:R19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="D11" sqref="C3:R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -961,10 +961,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:R19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
-      <selection sqref="A1:A19"/>
+    <sheetView zoomScale="61" workbookViewId="0">
+      <selection activeCell="F9" sqref="A1:R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -973,7 +973,11 @@
     <col min="3" max="18" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A1" t="str">
+        <f>IF(ISNUMBER(Mask!A1),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B1" t="str">
         <f>IF(ISNUMBER(Mask!B1),setup!$F$1,"")</f>
         <v/>
@@ -1043,7 +1047,11 @@
         <v/>
       </c>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" t="str">
+        <f>IF(ISNUMBER(Mask!A2),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B2" t="str">
         <f>IF(ISNUMBER(Mask!B2),setup!$F$1,"")</f>
         <v/>
@@ -1113,7 +1121,11 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" t="str">
+        <f>IF(ISNUMBER(Mask!A3),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B3" t="str">
         <f>IF(ISNUMBER(Mask!B3),setup!$F$1,"")</f>
         <v/>
@@ -1183,7 +1195,11 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" t="str">
+        <f>IF(ISNUMBER(Mask!A4),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B4" t="str">
         <f>IF(ISNUMBER(Mask!B4),setup!$F$1,"")</f>
         <v/>
@@ -1210,7 +1226,7 @@
       </c>
       <c r="H4" t="str">
         <f>IF(ISNUMBER(Mask!H4),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="I4" t="str">
         <f>IF(ISNUMBER(Mask!I4),setup!$F$1,"")</f>
@@ -1218,19 +1234,19 @@
       </c>
       <c r="J4" t="str">
         <f>IF(ISNUMBER(Mask!J4),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="K4" t="str">
         <f>IF(ISNUMBER(Mask!K4),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="L4" t="str">
         <f>IF(ISNUMBER(Mask!L4),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="M4" t="str">
         <f>IF(ISNUMBER(Mask!M4),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="N4" t="str">
         <f>IF(ISNUMBER(Mask!N4),setup!$F$1,"")</f>
@@ -1253,7 +1269,11 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" t="str">
+        <f>IF(ISNUMBER(Mask!A5),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B5" t="str">
         <f>IF(ISNUMBER(Mask!B5),setup!$F$1,"")</f>
         <v/>
@@ -1268,47 +1288,47 @@
       </c>
       <c r="E5" t="str">
         <f>IF(ISNUMBER(Mask!E5),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="F5" t="str">
         <f>IF(ISNUMBER(Mask!F5),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="G5" t="str">
         <f>IF(ISNUMBER(Mask!G5),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="H5" t="str">
         <f>IF(ISNUMBER(Mask!H5),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="I5" t="str">
         <f>IF(ISNUMBER(Mask!I5),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="J5" t="str">
         <f>IF(ISNUMBER(Mask!J5),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="K5" t="str">
         <f>IF(ISNUMBER(Mask!K5),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="L5" t="str">
         <f>IF(ISNUMBER(Mask!L5),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="M5" t="str">
         <f>IF(ISNUMBER(Mask!M5),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="N5" t="str">
         <f>IF(ISNUMBER(Mask!N5),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="O5" t="str">
         <f>IF(ISNUMBER(Mask!O5),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="P5" t="str">
         <f>IF(ISNUMBER(Mask!P5),setup!$F$1,"")</f>
@@ -1323,7 +1343,11 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" t="str">
+        <f>IF(ISNUMBER(Mask!A6),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B6" t="str">
         <f>IF(ISNUMBER(Mask!B6),setup!$F$1,"")</f>
         <v/>
@@ -1334,55 +1358,55 @@
       </c>
       <c r="D6" t="str">
         <f>IF(ISNUMBER(Mask!D6),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="E6" t="str">
         <f>IF(ISNUMBER(Mask!E6),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="F6" t="str">
         <f>IF(ISNUMBER(Mask!F6),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="G6" t="str">
         <f>IF(ISNUMBER(Mask!G6),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="H6" t="str">
         <f>IF(ISNUMBER(Mask!H6),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="I6" t="str">
         <f>IF(ISNUMBER(Mask!I6),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="J6" t="str">
         <f>IF(ISNUMBER(Mask!J6),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="K6" t="str">
         <f>IF(ISNUMBER(Mask!K6),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="L6" t="str">
         <f>IF(ISNUMBER(Mask!L6),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="M6" t="str">
         <f>IF(ISNUMBER(Mask!M6),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="N6" t="str">
         <f>IF(ISNUMBER(Mask!N6),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="O6" t="str">
         <f>IF(ISNUMBER(Mask!O6),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="P6" t="str">
         <f>IF(ISNUMBER(Mask!P6),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="Q6" t="str">
         <f>IF(ISNUMBER(Mask!Q6),setup!$F$1,"")</f>
@@ -1393,294 +1417,314 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" t="str">
+        <f>IF(ISNUMBER(Mask!A7),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B7" t="str">
         <f>IF(ISNUMBER(Mask!B7),setup!$F$1,"")</f>
         <v/>
       </c>
       <c r="C7" t="str">
         <f>IF(ISNUMBER(Mask!C7),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="D7" t="str">
         <f>IF(ISNUMBER(Mask!D7),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="E7" t="str">
         <f>IF(ISNUMBER(Mask!E7),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="F7" t="str">
         <f>IF(ISNUMBER(Mask!F7),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="G7" t="str">
         <f>IF(ISNUMBER(Mask!G7),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="H7" t="str">
         <f>IF(ISNUMBER(Mask!H7),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="I7" t="str">
         <f>IF(ISNUMBER(Mask!I7),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="J7" t="str">
         <f>IF(ISNUMBER(Mask!J7),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="K7" t="str">
         <f>IF(ISNUMBER(Mask!K7),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="L7" t="str">
         <f>IF(ISNUMBER(Mask!L7),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="M7" t="str">
         <f>IF(ISNUMBER(Mask!M7),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="N7" t="str">
         <f>IF(ISNUMBER(Mask!N7),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="O7" t="str">
         <f>IF(ISNUMBER(Mask!O7),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="P7" t="str">
         <f>IF(ISNUMBER(Mask!P7),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="Q7" t="str">
         <f>IF(ISNUMBER(Mask!Q7),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="R7" t="str">
         <f>IF(ISNUMBER(Mask!R7),setup!$F$1,"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" t="str">
+        <f>IF(ISNUMBER(Mask!A8),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B8" t="str">
         <f>IF(ISNUMBER(Mask!B8),setup!$F$1,"")</f>
         <v/>
       </c>
       <c r="C8" t="str">
         <f>IF(ISNUMBER(Mask!C8),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="D8" t="str">
         <f>IF(ISNUMBER(Mask!D8),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="E8" t="str">
         <f>IF(ISNUMBER(Mask!E8),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="F8" t="str">
         <f>IF(ISNUMBER(Mask!F8),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="G8" t="str">
         <f>IF(ISNUMBER(Mask!G8),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="H8" t="str">
         <f>IF(ISNUMBER(Mask!H8),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="I8" t="str">
         <f>IF(ISNUMBER(Mask!I8),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="J8" t="str">
         <f>IF(ISNUMBER(Mask!J8),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="K8" t="str">
         <f>IF(ISNUMBER(Mask!K8),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="L8" t="str">
         <f>IF(ISNUMBER(Mask!L8),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="M8" t="str">
         <f>IF(ISNUMBER(Mask!M8),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="N8" t="str">
         <f>IF(ISNUMBER(Mask!N8),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="O8" t="str">
         <f>IF(ISNUMBER(Mask!O8),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="P8" t="str">
         <f>IF(ISNUMBER(Mask!P8),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="Q8" t="str">
         <f>IF(ISNUMBER(Mask!Q8),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="R8" t="str">
         <f>IF(ISNUMBER(Mask!R8),setup!$F$1,"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" t="str">
+        <f>IF(ISNUMBER(Mask!A9),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B9" t="str">
         <f>IF(ISNUMBER(Mask!B9),setup!$F$1,"")</f>
         <v/>
       </c>
       <c r="C9" t="str">
         <f>IF(ISNUMBER(Mask!C9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="D9" t="str">
         <f>IF(ISNUMBER(Mask!D9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="E9" t="str">
         <f>IF(ISNUMBER(Mask!E9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="F9" t="str">
         <f>IF(ISNUMBER(Mask!F9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="G9" t="str">
         <f>IF(ISNUMBER(Mask!G9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="H9" t="str">
         <f>IF(ISNUMBER(Mask!H9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="I9" t="str">
         <f>IF(ISNUMBER(Mask!I9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="J9" t="str">
         <f>IF(ISNUMBER(Mask!J9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="K9" t="str">
         <f>IF(ISNUMBER(Mask!K9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="L9" t="str">
         <f>IF(ISNUMBER(Mask!L9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="M9" t="str">
         <f>IF(ISNUMBER(Mask!M9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="N9" t="str">
         <f>IF(ISNUMBER(Mask!N9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="O9" t="str">
         <f>IF(ISNUMBER(Mask!O9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="P9" t="str">
         <f>IF(ISNUMBER(Mask!P9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="Q9" t="str">
         <f>IF(ISNUMBER(Mask!Q9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="R9" t="str">
         <f>IF(ISNUMBER(Mask!R9),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
+        <v>100,100,100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" t="str">
+        <f>IF(ISNUMBER(Mask!A10),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B10" t="str">
         <f>IF(ISNUMBER(Mask!B10),setup!$F$1,"")</f>
         <v/>
       </c>
       <c r="C10" t="str">
         <f>IF(ISNUMBER(Mask!C10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="D10" t="str">
         <f>IF(ISNUMBER(Mask!D10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="E10" t="str">
         <f>IF(ISNUMBER(Mask!E10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="F10" t="str">
         <f>IF(ISNUMBER(Mask!F10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="G10" t="str">
         <f>IF(ISNUMBER(Mask!G10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="H10" t="str">
         <f>IF(ISNUMBER(Mask!H10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="I10" t="str">
         <f>IF(ISNUMBER(Mask!I10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="J10" t="str">
         <f>IF(ISNUMBER(Mask!J10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="K10" t="str">
         <f>IF(ISNUMBER(Mask!K10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="L10" t="str">
         <f>IF(ISNUMBER(Mask!L10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="M10" t="str">
         <f>IF(ISNUMBER(Mask!M10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="N10" t="str">
         <f>IF(ISNUMBER(Mask!N10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="O10" t="str">
         <f>IF(ISNUMBER(Mask!O10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="P10" t="str">
         <f>IF(ISNUMBER(Mask!P10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="Q10" t="str">
         <f>IF(ISNUMBER(Mask!Q10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="R10" t="str">
         <f>IF(ISNUMBER(Mask!R10),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
+        <v>100,100,100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" t="str">
+        <f>IF(ISNUMBER(Mask!A11),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B11" t="str">
         <f>IF(ISNUMBER(Mask!B11),setup!$F$1,"")</f>
         <v/>
       </c>
       <c r="C11" t="str">
         <f>IF(ISNUMBER(Mask!C11),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="D11" t="str">
         <f>IF(ISNUMBER(Mask!D11),setup!$F$1,"")</f>
@@ -1743,34 +1787,38 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" t="str">
+        <f>IF(ISNUMBER(Mask!A12),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B12" t="str">
         <f>IF(ISNUMBER(Mask!B12),setup!$F$1,"")</f>
         <v/>
       </c>
       <c r="C12" t="str">
         <f>IF(ISNUMBER(Mask!C12),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="D12" t="str">
         <f>IF(ISNUMBER(Mask!D12),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="E12" t="str">
         <f>IF(ISNUMBER(Mask!E12),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="F12" t="str">
         <f>IF(ISNUMBER(Mask!F12),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="G12" t="str">
         <f>IF(ISNUMBER(Mask!G12),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="H12" t="str">
         <f>IF(ISNUMBER(Mask!H12),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="I12" t="str">
         <f>IF(ISNUMBER(Mask!I12),setup!$F$1,"")</f>
@@ -1778,11 +1826,11 @@
       </c>
       <c r="J12" t="str">
         <f>IF(ISNUMBER(Mask!J12),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="K12" t="str">
         <f>IF(ISNUMBER(Mask!K12),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="L12" t="str">
         <f>IF(ISNUMBER(Mask!L12),setup!$F$1,"")</f>
@@ -1790,57 +1838,61 @@
       </c>
       <c r="M12" t="str">
         <f>IF(ISNUMBER(Mask!M12),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="N12" t="str">
         <f>IF(ISNUMBER(Mask!N12),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="O12" t="str">
         <f>IF(ISNUMBER(Mask!O12),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="P12" t="str">
         <f>IF(ISNUMBER(Mask!P12),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="Q12" t="str">
         <f>IF(ISNUMBER(Mask!Q12),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="R12" t="str">
         <f>IF(ISNUMBER(Mask!R12),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
+        <v>100,100,100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" t="str">
+        <f>IF(ISNUMBER(Mask!A13),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B13" t="str">
         <f>IF(ISNUMBER(Mask!B13),setup!$F$1,"")</f>
         <v/>
       </c>
       <c r="C13" t="str">
         <f>IF(ISNUMBER(Mask!C13),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="D13" t="str">
         <f>IF(ISNUMBER(Mask!D13),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="E13" t="str">
         <f>IF(ISNUMBER(Mask!E13),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="F13" t="str">
         <f>IF(ISNUMBER(Mask!F13),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="G13" t="str">
         <f>IF(ISNUMBER(Mask!G13),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="H13" t="str">
         <f>IF(ISNUMBER(Mask!H13),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="I13" t="str">
         <f>IF(ISNUMBER(Mask!I13),setup!$F$1,"")</f>
@@ -1848,11 +1900,11 @@
       </c>
       <c r="J13" t="str">
         <f>IF(ISNUMBER(Mask!J13),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="K13" t="str">
         <f>IF(ISNUMBER(Mask!K13),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="L13" t="str">
         <f>IF(ISNUMBER(Mask!L13),setup!$F$1,"")</f>
@@ -1860,57 +1912,61 @@
       </c>
       <c r="M13" t="str">
         <f>IF(ISNUMBER(Mask!M13),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="N13" t="str">
         <f>IF(ISNUMBER(Mask!N13),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="O13" t="str">
         <f>IF(ISNUMBER(Mask!O13),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="P13" t="str">
         <f>IF(ISNUMBER(Mask!P13),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="Q13" t="str">
         <f>IF(ISNUMBER(Mask!Q13),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="R13" t="str">
         <f>IF(ISNUMBER(Mask!R13),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
+        <v>100,100,100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" t="str">
+        <f>IF(ISNUMBER(Mask!A14),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B14" t="str">
         <f>IF(ISNUMBER(Mask!B14),setup!$F$1,"")</f>
         <v/>
       </c>
       <c r="C14" t="str">
         <f>IF(ISNUMBER(Mask!C14),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="D14" t="str">
         <f>IF(ISNUMBER(Mask!D14),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="E14" t="str">
         <f>IF(ISNUMBER(Mask!E14),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="F14" t="str">
         <f>IF(ISNUMBER(Mask!F14),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="G14" t="str">
         <f>IF(ISNUMBER(Mask!G14),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="H14" t="str">
         <f>IF(ISNUMBER(Mask!H14),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="I14" t="str">
         <f>IF(ISNUMBER(Mask!I14),setup!$F$1,"")</f>
@@ -1918,11 +1974,11 @@
       </c>
       <c r="J14" t="str">
         <f>IF(ISNUMBER(Mask!J14),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="K14" t="str">
         <f>IF(ISNUMBER(Mask!K14),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="L14" t="str">
         <f>IF(ISNUMBER(Mask!L14),setup!$F$1,"")</f>
@@ -1930,57 +1986,61 @@
       </c>
       <c r="M14" t="str">
         <f>IF(ISNUMBER(Mask!M14),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="N14" t="str">
         <f>IF(ISNUMBER(Mask!N14),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="O14" t="str">
         <f>IF(ISNUMBER(Mask!O14),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="P14" t="str">
         <f>IF(ISNUMBER(Mask!P14),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="Q14" t="str">
         <f>IF(ISNUMBER(Mask!Q14),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="R14" t="str">
         <f>IF(ISNUMBER(Mask!R14),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
+        <v>100,100,100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" t="str">
+        <f>IF(ISNUMBER(Mask!A15),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B15" t="str">
         <f>IF(ISNUMBER(Mask!B15),setup!$F$1,"")</f>
         <v/>
       </c>
       <c r="C15" t="str">
         <f>IF(ISNUMBER(Mask!C15),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="D15" t="str">
         <f>IF(ISNUMBER(Mask!D15),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="E15" t="str">
         <f>IF(ISNUMBER(Mask!E15),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="F15" t="str">
         <f>IF(ISNUMBER(Mask!F15),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="G15" t="str">
         <f>IF(ISNUMBER(Mask!G15),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="H15" t="str">
         <f>IF(ISNUMBER(Mask!H15),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="I15" t="str">
         <f>IF(ISNUMBER(Mask!I15),setup!$F$1,"")</f>
@@ -1988,11 +2048,11 @@
       </c>
       <c r="J15" t="str">
         <f>IF(ISNUMBER(Mask!J15),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="K15" t="str">
         <f>IF(ISNUMBER(Mask!K15),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="L15" t="str">
         <f>IF(ISNUMBER(Mask!L15),setup!$F$1,"")</f>
@@ -2000,30 +2060,34 @@
       </c>
       <c r="M15" t="str">
         <f>IF(ISNUMBER(Mask!M15),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="N15" t="str">
         <f>IF(ISNUMBER(Mask!N15),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="O15" t="str">
         <f>IF(ISNUMBER(Mask!O15),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="P15" t="str">
         <f>IF(ISNUMBER(Mask!P15),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="Q15" t="str">
         <f>IF(ISNUMBER(Mask!Q15),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="R15" t="str">
         <f>IF(ISNUMBER(Mask!R15),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.35">
+        <v>100,100,100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" t="str">
+        <f>IF(ISNUMBER(Mask!A16),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B16" t="str">
         <f>IF(ISNUMBER(Mask!B16),setup!$F$1,"")</f>
         <v/>
@@ -2046,11 +2110,11 @@
       </c>
       <c r="G16" t="str">
         <f>IF(ISNUMBER(Mask!G16),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="H16" t="str">
         <f>IF(ISNUMBER(Mask!H16),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="I16" t="str">
         <f>IF(ISNUMBER(Mask!I16),setup!$F$1,"")</f>
@@ -2058,11 +2122,11 @@
       </c>
       <c r="J16" t="str">
         <f>IF(ISNUMBER(Mask!J16),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="K16" t="str">
         <f>IF(ISNUMBER(Mask!K16),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="L16" t="str">
         <f>IF(ISNUMBER(Mask!L16),setup!$F$1,"")</f>
@@ -2070,30 +2134,34 @@
       </c>
       <c r="M16" t="str">
         <f>IF(ISNUMBER(Mask!M16),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="N16" t="str">
         <f>IF(ISNUMBER(Mask!N16),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="O16" t="str">
         <f>IF(ISNUMBER(Mask!O16),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="P16" t="str">
         <f>IF(ISNUMBER(Mask!P16),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="Q16" t="str">
         <f>IF(ISNUMBER(Mask!Q16),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="R16" t="str">
         <f>IF(ISNUMBER(Mask!R16),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
-      </c>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
+        <v>100,100,100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" t="str">
+        <f>IF(ISNUMBER(Mask!A17),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B17" t="str">
         <f>IF(ISNUMBER(Mask!B17),setup!$F$1,"")</f>
         <v/>
@@ -2120,7 +2188,7 @@
       </c>
       <c r="H17" t="str">
         <f>IF(ISNUMBER(Mask!H17),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="I17" t="str">
         <f>IF(ISNUMBER(Mask!I17),setup!$F$1,"")</f>
@@ -2128,11 +2196,11 @@
       </c>
       <c r="J17" t="str">
         <f>IF(ISNUMBER(Mask!J17),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="K17" t="str">
         <f>IF(ISNUMBER(Mask!K17),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="L17" t="str">
         <f>IF(ISNUMBER(Mask!L17),setup!$F$1,"")</f>
@@ -2140,7 +2208,7 @@
       </c>
       <c r="M17" t="str">
         <f>IF(ISNUMBER(Mask!M17),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="N17" t="str">
         <f>IF(ISNUMBER(Mask!N17),setup!$F$1,"")</f>
@@ -2163,7 +2231,11 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18" t="str">
+        <f>IF(ISNUMBER(Mask!A18),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B18" t="str">
         <f>IF(ISNUMBER(Mask!B18),setup!$F$1,"")</f>
         <v/>
@@ -2198,11 +2270,11 @@
       </c>
       <c r="J18" t="str">
         <f>IF(ISNUMBER(Mask!J18),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="K18" t="str">
         <f>IF(ISNUMBER(Mask!K18),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="L18" t="str">
         <f>IF(ISNUMBER(Mask!L18),setup!$F$1,"")</f>
@@ -2233,7 +2305,11 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A19" t="str">
+        <f>IF(ISNUMBER(Mask!A19),setup!$F$1,"")</f>
+        <v/>
+      </c>
       <c r="B19" t="str">
         <f>IF(ISNUMBER(Mask!B19),setup!$F$1,"")</f>
         <v/>
@@ -2268,11 +2344,11 @@
       </c>
       <c r="J19" t="str">
         <f>IF(ISNUMBER(Mask!J19),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="K19" t="str">
         <f>IF(ISNUMBER(Mask!K19),setup!$F$1,"")</f>
-        <v>(100,100,100)</v>
+        <v>100,100,100</v>
       </c>
       <c r="L19" t="str">
         <f>IF(ISNUMBER(Mask!L19),setup!$F$1,"")</f>
@@ -2314,7 +2390,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="A1:U21"/>
+      <selection sqref="A1:R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3692,15 +3768,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF6F8B5-AF9A-4C54-8212-EFBD25DA246B}">
-  <dimension ref="B1:R19"/>
+  <dimension ref="B1:S19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -3752,8 +3828,11 @@
       <c r="R1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -3805,8 +3884,11 @@
       <c r="R2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -3858,8 +3940,11 @@
       <c r="R3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -3879,13 +3964,13 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4" t="s">
         <v>3</v>
@@ -3897,7 +3982,7 @@
         <v>3</v>
       </c>
       <c r="N4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O4" t="s">
         <v>2</v>
@@ -3911,8 +3996,11 @@
       <c r="R4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -3923,7 +4011,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -3956,7 +4044,7 @@
         <v>3</v>
       </c>
       <c r="P5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q5" t="s">
         <v>2</v>
@@ -3964,8 +4052,11 @@
       <c r="R5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -3973,7 +4064,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
@@ -4012,18 +4103,21 @@
         <v>3</v>
       </c>
       <c r="Q6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -4068,15 +4162,18 @@
         <v>3</v>
       </c>
       <c r="R7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="S7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
@@ -4121,15 +4218,18 @@
         <v>3</v>
       </c>
       <c r="R8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="S8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
@@ -4176,13 +4276,16 @@
       <c r="R9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
         <v>3</v>
@@ -4229,16 +4332,19 @@
       <c r="R10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
@@ -4282,13 +4388,16 @@
       <c r="R11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
         <v>3</v>
@@ -4306,19 +4415,19 @@
         <v>3</v>
       </c>
       <c r="I12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K12" t="s">
         <v>3</v>
       </c>
       <c r="L12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N12" t="s">
         <v>3</v>
@@ -4335,13 +4444,16 @@
       <c r="R12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
         <v>3</v>
@@ -4359,19 +4471,19 @@
         <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K13" t="s">
         <v>3</v>
       </c>
       <c r="L13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N13" t="s">
         <v>3</v>
@@ -4388,13 +4500,16 @@
       <c r="R13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
         <v>3</v>
@@ -4412,19 +4527,19 @@
         <v>3</v>
       </c>
       <c r="I14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K14" t="s">
         <v>3</v>
       </c>
       <c r="L14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N14" t="s">
         <v>3</v>
@@ -4441,13 +4556,16 @@
       <c r="R14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
         <v>3</v>
@@ -4465,19 +4583,19 @@
         <v>3</v>
       </c>
       <c r="I15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K15" t="s">
         <v>3</v>
       </c>
       <c r="L15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N15" t="s">
         <v>3</v>
@@ -4494,8 +4612,11 @@
       <c r="R15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>2</v>
       </c>
@@ -4512,25 +4633,25 @@
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H16" t="s">
         <v>3</v>
       </c>
       <c r="I16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K16" t="s">
         <v>3</v>
       </c>
       <c r="L16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N16" t="s">
         <v>3</v>
@@ -4547,8 +4668,11 @@
       <c r="R16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -4568,25 +4692,25 @@
         <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K17" t="s">
         <v>3</v>
       </c>
       <c r="L17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O17" t="s">
         <v>2</v>
@@ -4600,8 +4724,11 @@
       <c r="R17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>2</v>
       </c>
@@ -4627,13 +4754,13 @@
         <v>2</v>
       </c>
       <c r="J18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K18" t="s">
         <v>3</v>
       </c>
       <c r="L18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M18" t="s">
         <v>2</v>
@@ -4653,8 +4780,11 @@
       <c r="R18" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="S18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>2</v>
       </c>
@@ -4680,13 +4810,13 @@
         <v>2</v>
       </c>
       <c r="J19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K19" t="s">
         <v>3</v>
       </c>
       <c r="L19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M19" t="s">
         <v>2</v>
@@ -4704,6 +4834,9 @@
         <v>2</v>
       </c>
       <c r="R19" t="s">
+        <v>2</v>
+      </c>
+      <c r="S19" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated excel for face
</commit_message>
<xml_diff>
--- a/blinka/data/grid.xlsx
+++ b/blinka/data/grid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\william.harding\Documents\repos\raspberrypi\blinka\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC29CE1F-C922-443F-80AA-733CB9B01D64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B5FAB0-BCB7-49E2-AB3D-A54CA1474041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="setup" sheetId="3" r:id="rId1"/>
@@ -38,12 +38,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="7">
   <si>
     <t>default color</t>
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>100,100,100</t>
+  </si>
+  <si>
+    <t>138,3,3</t>
+  </si>
+  <si>
+    <t>Blood Red</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>255,204,0</t>
   </si>
 </sst>
 </file>
@@ -361,16 +376,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E242987D-38C2-48DA-AD7C-35CC8D4AFA83}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.26953125" customWidth="1"/>
     <col min="2" max="4" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -387,9 +403,30 @@
       <c r="D1">
         <v>100</v>
       </c>
-      <c r="F1" t="str">
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="str">
         <f>B1&amp;","&amp;C1&amp;","&amp;D1</f>
         <v>100,100,100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1072,7 +1109,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView zoomScale="61" workbookViewId="0">
-      <selection activeCell="E8" sqref="A1:S20"/>
+      <selection activeCell="F16" sqref="A1:S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1313,7 +1350,7 @@
       </c>
       <c r="H4" t="str">
         <f>IF(ISNUMBER(Mask!H4),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I4" t="str">
         <f>IF(ISNUMBER(Mask!I4),setup!$F$1,"")</f>
@@ -1321,19 +1358,19 @@
       </c>
       <c r="J4" t="str">
         <f>IF(ISNUMBER(Mask!J4),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K4" t="str">
         <f>IF(ISNUMBER(Mask!K4),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L4" t="str">
         <f>IF(ISNUMBER(Mask!L4),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="M4" t="str">
         <f>IF(ISNUMBER(Mask!M4),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N4" t="str">
         <f>IF(ISNUMBER(Mask!N4),setup!$F$1,"")</f>
@@ -1374,47 +1411,47 @@
       </c>
       <c r="E5" t="str">
         <f>IF(ISNUMBER(Mask!E5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F5" t="str">
         <f>IF(ISNUMBER(Mask!F5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G5" t="str">
         <f>IF(ISNUMBER(Mask!G5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H5" t="str">
         <f>IF(ISNUMBER(Mask!H5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I5" t="str">
         <f>IF(ISNUMBER(Mask!I5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="J5" t="str">
         <f>IF(ISNUMBER(Mask!J5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K5" t="str">
         <f>IF(ISNUMBER(Mask!K5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L5" t="str">
         <f>IF(ISNUMBER(Mask!L5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="M5" t="str">
         <f>IF(ISNUMBER(Mask!M5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N5" t="str">
         <f>IF(ISNUMBER(Mask!N5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O5" t="str">
         <f>IF(ISNUMBER(Mask!O5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P5" t="str">
         <f>IF(ISNUMBER(Mask!P5),setup!$F$1,"")</f>
@@ -1443,55 +1480,55 @@
       </c>
       <c r="D6" t="str">
         <f>IF(ISNUMBER(Mask!D6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E6" t="str">
         <f>IF(ISNUMBER(Mask!E6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F6" t="str">
         <f>IF(ISNUMBER(Mask!F6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G6" t="str">
         <f>IF(ISNUMBER(Mask!G6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H6" t="str">
         <f>IF(ISNUMBER(Mask!H6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I6" t="str">
         <f>IF(ISNUMBER(Mask!I6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="J6" t="str">
         <f>IF(ISNUMBER(Mask!J6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K6" t="str">
         <f>IF(ISNUMBER(Mask!K6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L6" t="str">
         <f>IF(ISNUMBER(Mask!L6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="M6" t="str">
         <f>IF(ISNUMBER(Mask!M6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N6" t="str">
         <f>IF(ISNUMBER(Mask!N6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O6" t="str">
         <f>IF(ISNUMBER(Mask!O6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P6" t="str">
         <f>IF(ISNUMBER(Mask!P6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q6" t="str">
         <f>IF(ISNUMBER(Mask!Q6),setup!$F$1,"")</f>
@@ -1512,63 +1549,63 @@
       </c>
       <c r="C7" t="str">
         <f>IF(ISNUMBER(Mask!C7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D7" t="str">
         <f>IF(ISNUMBER(Mask!D7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E7" t="str">
         <f>IF(ISNUMBER(Mask!E7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F7" t="str">
         <f>IF(ISNUMBER(Mask!F7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G7" t="str">
         <f>IF(ISNUMBER(Mask!G7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H7" t="str">
         <f>IF(ISNUMBER(Mask!H7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I7" t="str">
         <f>IF(ISNUMBER(Mask!I7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="J7" t="str">
         <f>IF(ISNUMBER(Mask!J7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K7" t="str">
         <f>IF(ISNUMBER(Mask!K7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L7" t="str">
         <f>IF(ISNUMBER(Mask!L7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="M7" t="str">
         <f>IF(ISNUMBER(Mask!M7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N7" t="str">
         <f>IF(ISNUMBER(Mask!N7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O7" t="str">
         <f>IF(ISNUMBER(Mask!O7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P7" t="str">
         <f>IF(ISNUMBER(Mask!P7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q7" t="str">
         <f>IF(ISNUMBER(Mask!Q7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R7" t="str">
         <f>IF(ISNUMBER(Mask!R7),setup!$F$1,"")</f>
@@ -1585,63 +1622,63 @@
       </c>
       <c r="C8" t="str">
         <f>IF(ISNUMBER(Mask!C8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D8" t="str">
         <f>IF(ISNUMBER(Mask!D8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E8" t="str">
         <f>IF(ISNUMBER(Mask!E8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F8" t="str">
         <f>IF(ISNUMBER(Mask!F8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G8" t="str">
         <f>IF(ISNUMBER(Mask!G8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H8" t="str">
         <f>IF(ISNUMBER(Mask!H8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I8" t="str">
         <f>IF(ISNUMBER(Mask!I8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="J8" t="str">
         <f>IF(ISNUMBER(Mask!J8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K8" t="str">
         <f>IF(ISNUMBER(Mask!K8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L8" t="str">
         <f>IF(ISNUMBER(Mask!L8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="M8" t="str">
         <f>IF(ISNUMBER(Mask!M8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N8" t="str">
         <f>IF(ISNUMBER(Mask!N8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O8" t="str">
         <f>IF(ISNUMBER(Mask!O8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P8" t="str">
         <f>IF(ISNUMBER(Mask!P8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q8" t="str">
         <f>IF(ISNUMBER(Mask!Q8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R8" t="str">
         <f>IF(ISNUMBER(Mask!R8),setup!$F$1,"")</f>
@@ -1658,67 +1695,67 @@
       </c>
       <c r="C9" t="str">
         <f>IF(ISNUMBER(Mask!C9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D9" t="str">
         <f>IF(ISNUMBER(Mask!D9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E9" t="str">
         <f>IF(ISNUMBER(Mask!E9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F9" t="str">
         <f>IF(ISNUMBER(Mask!F9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G9" t="str">
         <f>IF(ISNUMBER(Mask!G9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H9" t="str">
         <f>IF(ISNUMBER(Mask!H9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I9" t="str">
         <f>IF(ISNUMBER(Mask!I9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="J9" t="str">
         <f>IF(ISNUMBER(Mask!J9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K9" t="str">
         <f>IF(ISNUMBER(Mask!K9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L9" t="str">
         <f>IF(ISNUMBER(Mask!L9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="M9" t="str">
         <f>IF(ISNUMBER(Mask!M9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N9" t="str">
         <f>IF(ISNUMBER(Mask!N9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O9" t="str">
         <f>IF(ISNUMBER(Mask!O9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P9" t="str">
         <f>IF(ISNUMBER(Mask!P9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q9" t="str">
         <f>IF(ISNUMBER(Mask!Q9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R9" t="str">
         <f>IF(ISNUMBER(Mask!R9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
@@ -1731,67 +1768,67 @@
       </c>
       <c r="C10" t="str">
         <f>IF(ISNUMBER(Mask!C10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D10" t="str">
         <f>IF(ISNUMBER(Mask!D10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E10" t="str">
         <f>IF(ISNUMBER(Mask!E10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F10" t="str">
         <f>IF(ISNUMBER(Mask!F10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G10" t="str">
         <f>IF(ISNUMBER(Mask!G10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H10" t="str">
         <f>IF(ISNUMBER(Mask!H10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I10" t="str">
         <f>IF(ISNUMBER(Mask!I10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="J10" t="str">
         <f>IF(ISNUMBER(Mask!J10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K10" t="str">
         <f>IF(ISNUMBER(Mask!K10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L10" t="str">
         <f>IF(ISNUMBER(Mask!L10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="M10" t="str">
         <f>IF(ISNUMBER(Mask!M10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N10" t="str">
         <f>IF(ISNUMBER(Mask!N10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O10" t="str">
         <f>IF(ISNUMBER(Mask!O10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P10" t="str">
         <f>IF(ISNUMBER(Mask!P10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q10" t="str">
         <f>IF(ISNUMBER(Mask!Q10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R10" t="str">
         <f>IF(ISNUMBER(Mask!R10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
@@ -1804,7 +1841,7 @@
       </c>
       <c r="C11" t="str">
         <f>IF(ISNUMBER(Mask!C11),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D11" t="str">
         <f>IF(ISNUMBER(Mask!D11),setup!$F$1,"")</f>
@@ -1877,27 +1914,27 @@
       </c>
       <c r="C12" t="str">
         <f>IF(ISNUMBER(Mask!C12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D12" t="str">
         <f>IF(ISNUMBER(Mask!D12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E12" t="str">
         <f>IF(ISNUMBER(Mask!E12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F12" t="str">
         <f>IF(ISNUMBER(Mask!F12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G12" t="str">
         <f>IF(ISNUMBER(Mask!G12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H12" t="str">
         <f>IF(ISNUMBER(Mask!H12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I12" t="str">
         <f>IF(ISNUMBER(Mask!I12),setup!$F$1,"")</f>
@@ -1905,11 +1942,11 @@
       </c>
       <c r="J12" t="str">
         <f>IF(ISNUMBER(Mask!J12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K12" t="str">
         <f>IF(ISNUMBER(Mask!K12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L12" t="str">
         <f>IF(ISNUMBER(Mask!L12),setup!$F$1,"")</f>
@@ -1917,27 +1954,27 @@
       </c>
       <c r="M12" t="str">
         <f>IF(ISNUMBER(Mask!M12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N12" t="str">
         <f>IF(ISNUMBER(Mask!N12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O12" t="str">
         <f>IF(ISNUMBER(Mask!O12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P12" t="str">
         <f>IF(ISNUMBER(Mask!P12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q12" t="str">
         <f>IF(ISNUMBER(Mask!Q12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R12" t="str">
         <f>IF(ISNUMBER(Mask!R12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
@@ -1950,27 +1987,27 @@
       </c>
       <c r="C13" t="str">
         <f>IF(ISNUMBER(Mask!C13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D13" t="str">
         <f>IF(ISNUMBER(Mask!D13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E13" t="str">
         <f>IF(ISNUMBER(Mask!E13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F13" t="str">
         <f>IF(ISNUMBER(Mask!F13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G13" t="str">
         <f>IF(ISNUMBER(Mask!G13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H13" t="str">
         <f>IF(ISNUMBER(Mask!H13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I13" t="str">
         <f>IF(ISNUMBER(Mask!I13),setup!$F$1,"")</f>
@@ -1978,11 +2015,11 @@
       </c>
       <c r="J13" t="str">
         <f>IF(ISNUMBER(Mask!J13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K13" t="str">
         <f>IF(ISNUMBER(Mask!K13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L13" t="str">
         <f>IF(ISNUMBER(Mask!L13),setup!$F$1,"")</f>
@@ -1990,27 +2027,27 @@
       </c>
       <c r="M13" t="str">
         <f>IF(ISNUMBER(Mask!M13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N13" t="str">
         <f>IF(ISNUMBER(Mask!N13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O13" t="str">
         <f>IF(ISNUMBER(Mask!O13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P13" t="str">
         <f>IF(ISNUMBER(Mask!P13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q13" t="str">
         <f>IF(ISNUMBER(Mask!Q13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R13" t="str">
         <f>IF(ISNUMBER(Mask!R13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
@@ -2023,27 +2060,27 @@
       </c>
       <c r="C14" t="str">
         <f>IF(ISNUMBER(Mask!C14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D14" t="str">
         <f>IF(ISNUMBER(Mask!D14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E14" t="str">
         <f>IF(ISNUMBER(Mask!E14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F14" t="str">
         <f>IF(ISNUMBER(Mask!F14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G14" t="str">
         <f>IF(ISNUMBER(Mask!G14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H14" t="str">
         <f>IF(ISNUMBER(Mask!H14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I14" t="str">
         <f>IF(ISNUMBER(Mask!I14),setup!$F$1,"")</f>
@@ -2051,11 +2088,11 @@
       </c>
       <c r="J14" t="str">
         <f>IF(ISNUMBER(Mask!J14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K14" t="str">
         <f>IF(ISNUMBER(Mask!K14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L14" t="str">
         <f>IF(ISNUMBER(Mask!L14),setup!$F$1,"")</f>
@@ -2063,27 +2100,27 @@
       </c>
       <c r="M14" t="str">
         <f>IF(ISNUMBER(Mask!M14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N14" t="str">
         <f>IF(ISNUMBER(Mask!N14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O14" t="str">
         <f>IF(ISNUMBER(Mask!O14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P14" t="str">
         <f>IF(ISNUMBER(Mask!P14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q14" t="str">
         <f>IF(ISNUMBER(Mask!Q14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R14" t="str">
         <f>IF(ISNUMBER(Mask!R14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
@@ -2096,27 +2133,27 @@
       </c>
       <c r="C15" t="str">
         <f>IF(ISNUMBER(Mask!C15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D15" t="str">
         <f>IF(ISNUMBER(Mask!D15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E15" t="str">
         <f>IF(ISNUMBER(Mask!E15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F15" t="str">
         <f>IF(ISNUMBER(Mask!F15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G15" t="str">
         <f>IF(ISNUMBER(Mask!G15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H15" t="str">
         <f>IF(ISNUMBER(Mask!H15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I15" t="str">
         <f>IF(ISNUMBER(Mask!I15),setup!$F$1,"")</f>
@@ -2124,11 +2161,11 @@
       </c>
       <c r="J15" t="str">
         <f>IF(ISNUMBER(Mask!J15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K15" t="str">
         <f>IF(ISNUMBER(Mask!K15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L15" t="str">
         <f>IF(ISNUMBER(Mask!L15),setup!$F$1,"")</f>
@@ -2136,27 +2173,27 @@
       </c>
       <c r="M15" t="str">
         <f>IF(ISNUMBER(Mask!M15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N15" t="str">
         <f>IF(ISNUMBER(Mask!N15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O15" t="str">
         <f>IF(ISNUMBER(Mask!O15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P15" t="str">
         <f>IF(ISNUMBER(Mask!P15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q15" t="str">
         <f>IF(ISNUMBER(Mask!Q15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R15" t="str">
         <f>IF(ISNUMBER(Mask!R15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
@@ -2185,11 +2222,11 @@
       </c>
       <c r="G16" t="str">
         <f>IF(ISNUMBER(Mask!G16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H16" t="str">
         <f>IF(ISNUMBER(Mask!H16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I16" t="str">
         <f>IF(ISNUMBER(Mask!I16),setup!$F$1,"")</f>
@@ -2197,11 +2234,11 @@
       </c>
       <c r="J16" t="str">
         <f>IF(ISNUMBER(Mask!J16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K16" t="str">
         <f>IF(ISNUMBER(Mask!K16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L16" t="str">
         <f>IF(ISNUMBER(Mask!L16),setup!$F$1,"")</f>
@@ -2209,27 +2246,27 @@
       </c>
       <c r="M16" t="str">
         <f>IF(ISNUMBER(Mask!M16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N16" t="str">
         <f>IF(ISNUMBER(Mask!N16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O16" t="str">
         <f>IF(ISNUMBER(Mask!O16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P16" t="str">
         <f>IF(ISNUMBER(Mask!P16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q16" t="str">
         <f>IF(ISNUMBER(Mask!Q16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R16" t="str">
         <f>IF(ISNUMBER(Mask!R16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
@@ -2262,7 +2299,7 @@
       </c>
       <c r="H17" t="str">
         <f>IF(ISNUMBER(Mask!H17),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I17" t="str">
         <f>IF(ISNUMBER(Mask!I17),setup!$F$1,"")</f>
@@ -2270,11 +2307,11 @@
       </c>
       <c r="J17" t="str">
         <f>IF(ISNUMBER(Mask!J17),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K17" t="str">
         <f>IF(ISNUMBER(Mask!K17),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L17" t="str">
         <f>IF(ISNUMBER(Mask!L17),setup!$F$1,"")</f>
@@ -2282,7 +2319,7 @@
       </c>
       <c r="M17" t="str">
         <f>IF(ISNUMBER(Mask!M17),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N17" t="str">
         <f>IF(ISNUMBER(Mask!N17),setup!$F$1,"")</f>
@@ -2343,11 +2380,11 @@
       </c>
       <c r="J18" t="str">
         <f>IF(ISNUMBER(Mask!J18),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K18" t="str">
         <f>IF(ISNUMBER(Mask!K18),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L18" t="str">
         <f>IF(ISNUMBER(Mask!L18),setup!$F$1,"")</f>
@@ -2416,11 +2453,11 @@
       </c>
       <c r="J19" t="str">
         <f>IF(ISNUMBER(Mask!J19),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K19" t="str">
         <f>IF(ISNUMBER(Mask!K19),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L19" t="str">
         <f>IF(ISNUMBER(Mask!L19),setup!$F$1,"")</f>
@@ -2466,8 +2503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C3361C-1C15-4A97-8B76-564436F68EDA}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:S20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2538,73 +2575,56 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="H2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="I2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="K2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="L2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="N2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="O2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="P2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>1</v>
       </c>
       <c r="T2" t="s">
         <v>1</v>
@@ -2617,73 +2637,56 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="str">
-        <f>IF(ISNUMBER(Mask!B3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C3" t="str">
-        <f>IF(ISNUMBER(Mask!C3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D3" t="str">
-        <f>IF(ISNUMBER(Mask!D3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E3" t="str">
-        <f>IF(ISNUMBER(Mask!E3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F3" t="str">
-        <f>IF(ISNUMBER(Mask!F3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G3" t="str">
-        <f>IF(ISNUMBER(Mask!G3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="H3" t="str">
-        <f>IF(ISNUMBER(Mask!H3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="I3" t="str">
-        <f>IF(ISNUMBER(Mask!I3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J3" t="str">
-        <f>IF(ISNUMBER(Mask!J3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="K3" t="str">
-        <f>IF(ISNUMBER(Mask!K3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="L3" t="str">
-        <f>IF(ISNUMBER(Mask!L3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M3" t="str">
-        <f>IF(ISNUMBER(Mask!M3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="N3" t="str">
-        <f>IF(ISNUMBER(Mask!N3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="O3" t="str">
-        <f>IF(ISNUMBER(Mask!O3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="P3" t="str">
-        <f>IF(ISNUMBER(Mask!P3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q3" t="str">
-        <f>IF(ISNUMBER(Mask!Q3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R3" t="str">
-        <f>IF(ISNUMBER(Mask!R3),setup!$F$1,"")</f>
-        <v/>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>1</v>
       </c>
       <c r="T3" t="s">
         <v>1</v>
@@ -2696,73 +2699,56 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="str">
-        <f>IF(ISNUMBER(Mask!B4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C4" t="str">
-        <f>IF(ISNUMBER(Mask!C4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D4" t="str">
-        <f>IF(ISNUMBER(Mask!D4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E4" t="str">
-        <f>IF(ISNUMBER(Mask!E4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F4" t="str">
-        <f>IF(ISNUMBER(Mask!F4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G4" t="str">
-        <f>IF(ISNUMBER(Mask!G4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="H4" t="str">
-        <f>IF(ISNUMBER(Mask!H4),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="I4" t="str">
-        <f>IF(ISNUMBER(Mask!I4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J4" t="str">
-        <f>IF(ISNUMBER(Mask!J4),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="K4" t="str">
-        <f>IF(ISNUMBER(Mask!K4),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="L4" t="str">
-        <f>IF(ISNUMBER(Mask!L4),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="M4" t="str">
-        <f>IF(ISNUMBER(Mask!M4),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="N4" t="str">
-        <f>IF(ISNUMBER(Mask!N4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="O4" t="str">
-        <f>IF(ISNUMBER(Mask!O4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="P4" t="str">
-        <f>IF(ISNUMBER(Mask!P4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q4" t="str">
-        <f>IF(ISNUMBER(Mask!Q4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R4" t="str">
-        <f>IF(ISNUMBER(Mask!R4),setup!$F$1,"")</f>
-        <v/>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1</v>
       </c>
       <c r="T4" t="s">
         <v>1</v>
@@ -2775,73 +2761,56 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="str">
-        <f>IF(ISNUMBER(Mask!B5),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C5" t="str">
-        <f>IF(ISNUMBER(Mask!C5),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D5" t="str">
-        <f>IF(ISNUMBER(Mask!D5),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E5" t="str">
-        <f>IF(ISNUMBER(Mask!E5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="F5" t="str">
-        <f>IF(ISNUMBER(Mask!F5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="G5" t="str">
-        <f>IF(ISNUMBER(Mask!G5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="H5" t="str">
-        <f>IF(ISNUMBER(Mask!H5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="I5" t="str">
-        <f>IF(ISNUMBER(Mask!I5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="J5" t="str">
-        <f>IF(ISNUMBER(Mask!J5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="K5" t="str">
-        <f>IF(ISNUMBER(Mask!K5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="L5" t="str">
-        <f>IF(ISNUMBER(Mask!L5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="M5" t="str">
-        <f>IF(ISNUMBER(Mask!M5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="N5" t="str">
-        <f>IF(ISNUMBER(Mask!N5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="O5" t="str">
-        <f>IF(ISNUMBER(Mask!O5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="P5" t="str">
-        <f>IF(ISNUMBER(Mask!P5),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q5" t="str">
-        <f>IF(ISNUMBER(Mask!Q5),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R5" t="str">
-        <f>IF(ISNUMBER(Mask!R5),setup!$F$1,"")</f>
-        <v/>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>1</v>
       </c>
       <c r="T5" t="s">
         <v>1</v>
@@ -2854,73 +2823,56 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="str">
-        <f>IF(ISNUMBER(Mask!B6),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C6" t="str">
-        <f>IF(ISNUMBER(Mask!C6),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D6" t="str">
-        <f>IF(ISNUMBER(Mask!D6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="E6" t="str">
-        <f>IF(ISNUMBER(Mask!E6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="F6" t="str">
-        <f>IF(ISNUMBER(Mask!F6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="G6" t="str">
-        <f>IF(ISNUMBER(Mask!G6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="H6" t="str">
-        <f>IF(ISNUMBER(Mask!H6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="I6" t="str">
-        <f>IF(ISNUMBER(Mask!I6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="J6" t="str">
-        <f>IF(ISNUMBER(Mask!J6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="K6" t="str">
-        <f>IF(ISNUMBER(Mask!K6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="L6" t="str">
-        <f>IF(ISNUMBER(Mask!L6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="M6" t="str">
-        <f>IF(ISNUMBER(Mask!M6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="N6" t="str">
-        <f>IF(ISNUMBER(Mask!N6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="O6" t="str">
-        <f>IF(ISNUMBER(Mask!O6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="P6" t="str">
-        <f>IF(ISNUMBER(Mask!P6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="Q6" t="str">
-        <f>IF(ISNUMBER(Mask!Q6),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R6" t="str">
-        <f>IF(ISNUMBER(Mask!R6),setup!$F$1,"")</f>
-        <v/>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1</v>
       </c>
       <c r="T6" t="s">
         <v>1</v>
@@ -2933,73 +2885,56 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="str">
-        <f>IF(ISNUMBER(Mask!B7),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C7" t="str">
-        <f>IF(ISNUMBER(Mask!C7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="D7" t="str">
-        <f>IF(ISNUMBER(Mask!D7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="E7" t="str">
-        <f>IF(ISNUMBER(Mask!E7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="F7" t="str">
-        <f>IF(ISNUMBER(Mask!F7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="G7" t="str">
-        <f>IF(ISNUMBER(Mask!G7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="H7" t="str">
-        <f>IF(ISNUMBER(Mask!H7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="I7" t="str">
-        <f>IF(ISNUMBER(Mask!I7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="J7" t="str">
-        <f>IF(ISNUMBER(Mask!J7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="K7" t="str">
-        <f>IF(ISNUMBER(Mask!K7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="L7" t="str">
-        <f>IF(ISNUMBER(Mask!L7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="M7" t="str">
-        <f>IF(ISNUMBER(Mask!M7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="N7" t="str">
-        <f>IF(ISNUMBER(Mask!N7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="O7" t="str">
-        <f>IF(ISNUMBER(Mask!O7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="P7" t="str">
-        <f>IF(ISNUMBER(Mask!P7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="Q7" t="str">
-        <f>IF(ISNUMBER(Mask!Q7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="R7" t="str">
-        <f>IF(ISNUMBER(Mask!R7),setup!$F$1,"")</f>
-        <v/>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>3</v>
+      </c>
+      <c r="R7" t="s">
+        <v>1</v>
       </c>
       <c r="T7" t="s">
         <v>1</v>
@@ -3012,73 +2947,56 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="str">
-        <f>IF(ISNUMBER(Mask!B8),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C8" t="str">
-        <f>IF(ISNUMBER(Mask!C8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="D8" t="str">
-        <f>IF(ISNUMBER(Mask!D8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="E8" t="str">
-        <f>IF(ISNUMBER(Mask!E8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="F8" t="str">
-        <f>IF(ISNUMBER(Mask!F8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="G8" t="str">
-        <f>IF(ISNUMBER(Mask!G8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="H8" t="str">
-        <f>IF(ISNUMBER(Mask!H8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="I8" t="str">
-        <f>IF(ISNUMBER(Mask!I8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="J8" t="str">
-        <f>IF(ISNUMBER(Mask!J8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="K8" t="str">
-        <f>IF(ISNUMBER(Mask!K8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="L8" t="str">
-        <f>IF(ISNUMBER(Mask!L8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="M8" t="str">
-        <f>IF(ISNUMBER(Mask!M8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="N8" t="str">
-        <f>IF(ISNUMBER(Mask!N8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="O8" t="str">
-        <f>IF(ISNUMBER(Mask!O8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="P8" t="str">
-        <f>IF(ISNUMBER(Mask!P8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="Q8" t="str">
-        <f>IF(ISNUMBER(Mask!Q8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="R8" t="str">
-        <f>IF(ISNUMBER(Mask!R8),setup!$F$1,"")</f>
-        <v/>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R8" t="s">
+        <v>1</v>
       </c>
       <c r="T8" t="s">
         <v>1</v>
@@ -3091,73 +3009,56 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="str">
-        <f>IF(ISNUMBER(Mask!B9),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C9" t="str">
-        <f>IF(ISNUMBER(Mask!C9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="D9" t="str">
-        <f>IF(ISNUMBER(Mask!D9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="E9" t="str">
-        <f>IF(ISNUMBER(Mask!E9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="F9" t="str">
-        <f>IF(ISNUMBER(Mask!F9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="G9" t="str">
-        <f>IF(ISNUMBER(Mask!G9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="H9" t="str">
-        <f>IF(ISNUMBER(Mask!H9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="I9" t="str">
-        <f>IF(ISNUMBER(Mask!I9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="J9" t="str">
-        <f>IF(ISNUMBER(Mask!J9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="K9" t="str">
-        <f>IF(ISNUMBER(Mask!K9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="L9" t="str">
-        <f>IF(ISNUMBER(Mask!L9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="M9" t="str">
-        <f>IF(ISNUMBER(Mask!M9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="N9" t="str">
-        <f>IF(ISNUMBER(Mask!N9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="O9" t="str">
-        <f>IF(ISNUMBER(Mask!O9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="P9" t="str">
-        <f>IF(ISNUMBER(Mask!P9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="Q9" t="str">
-        <f>IF(ISNUMBER(Mask!Q9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="R9" t="str">
-        <f>IF(ISNUMBER(Mask!R9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>3</v>
+      </c>
+      <c r="R9" t="s">
+        <v>3</v>
       </c>
       <c r="T9" t="s">
         <v>1</v>
@@ -3170,73 +3071,56 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="str">
-        <f>IF(ISNUMBER(Mask!B10),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C10" t="str">
-        <f>IF(ISNUMBER(Mask!C10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="D10" t="str">
-        <f>IF(ISNUMBER(Mask!D10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="E10" t="str">
-        <f>IF(ISNUMBER(Mask!E10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="F10" t="str">
-        <f>IF(ISNUMBER(Mask!F10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="G10" t="str">
-        <f>IF(ISNUMBER(Mask!G10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="H10" t="str">
-        <f>IF(ISNUMBER(Mask!H10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="I10" t="str">
-        <f>IF(ISNUMBER(Mask!I10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="J10" t="str">
-        <f>IF(ISNUMBER(Mask!J10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="K10" t="str">
-        <f>IF(ISNUMBER(Mask!K10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="L10" t="str">
-        <f>IF(ISNUMBER(Mask!L10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="M10" t="str">
-        <f>IF(ISNUMBER(Mask!M10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="N10" t="str">
-        <f>IF(ISNUMBER(Mask!N10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="O10" t="str">
-        <f>IF(ISNUMBER(Mask!O10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="P10" t="str">
-        <f>IF(ISNUMBER(Mask!P10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="Q10" t="str">
-        <f>IF(ISNUMBER(Mask!Q10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="R10" t="str">
-        <f>IF(ISNUMBER(Mask!R10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N10" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>6</v>
+      </c>
+      <c r="R10" t="s">
+        <v>3</v>
       </c>
       <c r="T10" t="s">
         <v>1</v>
@@ -3249,73 +3133,56 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="str">
-        <f>IF(ISNUMBER(Mask!B11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C11" t="str">
-        <f>IF(ISNUMBER(Mask!C11),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="D11" t="str">
-        <f>IF(ISNUMBER(Mask!D11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E11" t="str">
-        <f>IF(ISNUMBER(Mask!E11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F11" t="str">
-        <f>IF(ISNUMBER(Mask!F11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G11" t="str">
-        <f>IF(ISNUMBER(Mask!G11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="H11" t="str">
-        <f>IF(ISNUMBER(Mask!H11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="I11" t="str">
-        <f>IF(ISNUMBER(Mask!I11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J11" t="str">
-        <f>IF(ISNUMBER(Mask!J11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="K11" t="str">
-        <f>IF(ISNUMBER(Mask!K11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="L11" t="str">
-        <f>IF(ISNUMBER(Mask!L11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M11" t="str">
-        <f>IF(ISNUMBER(Mask!M11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="N11" t="str">
-        <f>IF(ISNUMBER(Mask!N11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="O11" t="str">
-        <f>IF(ISNUMBER(Mask!O11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="P11" t="str">
-        <f>IF(ISNUMBER(Mask!P11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q11" t="str">
-        <f>IF(ISNUMBER(Mask!Q11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R11" t="str">
-        <f>IF(ISNUMBER(Mask!R11),setup!$F$1,"")</f>
-        <v/>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>1</v>
+      </c>
+      <c r="R11" t="s">
+        <v>1</v>
       </c>
       <c r="T11" t="s">
         <v>1</v>
@@ -3328,73 +3195,56 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="str">
-        <f>IF(ISNUMBER(Mask!B12),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C12" t="str">
-        <f>IF(ISNUMBER(Mask!C12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="D12" t="str">
-        <f>IF(ISNUMBER(Mask!D12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="E12" t="str">
-        <f>IF(ISNUMBER(Mask!E12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="F12" t="str">
-        <f>IF(ISNUMBER(Mask!F12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="G12" t="str">
-        <f>IF(ISNUMBER(Mask!G12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="H12" t="str">
-        <f>IF(ISNUMBER(Mask!H12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="I12" t="str">
-        <f>IF(ISNUMBER(Mask!I12),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J12" t="str">
-        <f>IF(ISNUMBER(Mask!J12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="K12" t="str">
-        <f>IF(ISNUMBER(Mask!K12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="L12" t="str">
-        <f>IF(ISNUMBER(Mask!L12),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M12" t="str">
-        <f>IF(ISNUMBER(Mask!M12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="N12" t="str">
-        <f>IF(ISNUMBER(Mask!N12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="O12" t="str">
-        <f>IF(ISNUMBER(Mask!O12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="P12" t="str">
-        <f>IF(ISNUMBER(Mask!P12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="Q12" t="str">
-        <f>IF(ISNUMBER(Mask!Q12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="R12" t="str">
-        <f>IF(ISNUMBER(Mask!R12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O12" t="s">
+        <v>6</v>
+      </c>
+      <c r="P12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>6</v>
+      </c>
+      <c r="R12" t="s">
+        <v>3</v>
       </c>
       <c r="T12" t="s">
         <v>1</v>
@@ -3407,73 +3257,56 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="str">
-        <f>IF(ISNUMBER(Mask!B13),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C13" t="str">
-        <f>IF(ISNUMBER(Mask!C13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="D13" t="str">
-        <f>IF(ISNUMBER(Mask!D13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="E13" t="str">
-        <f>IF(ISNUMBER(Mask!E13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="F13" t="str">
-        <f>IF(ISNUMBER(Mask!F13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="G13" t="str">
-        <f>IF(ISNUMBER(Mask!G13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="H13" t="str">
-        <f>IF(ISNUMBER(Mask!H13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="I13" t="str">
-        <f>IF(ISNUMBER(Mask!I13),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J13" t="str">
-        <f>IF(ISNUMBER(Mask!J13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="K13" t="str">
-        <f>IF(ISNUMBER(Mask!K13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="L13" t="str">
-        <f>IF(ISNUMBER(Mask!L13),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M13" t="str">
-        <f>IF(ISNUMBER(Mask!M13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="N13" t="str">
-        <f>IF(ISNUMBER(Mask!N13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="O13" t="str">
-        <f>IF(ISNUMBER(Mask!O13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="P13" t="str">
-        <f>IF(ISNUMBER(Mask!P13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="Q13" t="str">
-        <f>IF(ISNUMBER(Mask!Q13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="R13" t="str">
-        <f>IF(ISNUMBER(Mask!R13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13" t="s">
+        <v>3</v>
+      </c>
+      <c r="O13" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>3</v>
+      </c>
+      <c r="R13" t="s">
+        <v>3</v>
       </c>
       <c r="T13" t="s">
         <v>1</v>
@@ -3486,73 +3319,56 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="str">
-        <f>IF(ISNUMBER(Mask!B14),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C14" t="str">
-        <f>IF(ISNUMBER(Mask!C14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="D14" t="str">
-        <f>IF(ISNUMBER(Mask!D14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="E14" t="str">
-        <f>IF(ISNUMBER(Mask!E14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="F14" t="str">
-        <f>IF(ISNUMBER(Mask!F14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="G14" t="str">
-        <f>IF(ISNUMBER(Mask!G14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="H14" t="str">
-        <f>IF(ISNUMBER(Mask!H14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="I14" t="str">
-        <f>IF(ISNUMBER(Mask!I14),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J14" t="str">
-        <f>IF(ISNUMBER(Mask!J14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="K14" t="str">
-        <f>IF(ISNUMBER(Mask!K14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="L14" t="str">
-        <f>IF(ISNUMBER(Mask!L14),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M14" t="str">
-        <f>IF(ISNUMBER(Mask!M14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="N14" t="str">
-        <f>IF(ISNUMBER(Mask!N14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="O14" t="str">
-        <f>IF(ISNUMBER(Mask!O14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="P14" t="str">
-        <f>IF(ISNUMBER(Mask!P14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="Q14" t="str">
-        <f>IF(ISNUMBER(Mask!Q14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="R14" t="str">
-        <f>IF(ISNUMBER(Mask!R14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" t="s">
+        <v>3</v>
+      </c>
+      <c r="P14" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>3</v>
+      </c>
+      <c r="R14" t="s">
+        <v>3</v>
       </c>
       <c r="T14" t="s">
         <v>1</v>
@@ -3565,73 +3381,56 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="str">
-        <f>IF(ISNUMBER(Mask!B15),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C15" t="str">
-        <f>IF(ISNUMBER(Mask!C15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="D15" t="str">
-        <f>IF(ISNUMBER(Mask!D15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="E15" t="str">
-        <f>IF(ISNUMBER(Mask!E15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="F15" t="str">
-        <f>IF(ISNUMBER(Mask!F15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="G15" t="str">
-        <f>IF(ISNUMBER(Mask!G15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="H15" t="str">
-        <f>IF(ISNUMBER(Mask!H15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="I15" t="str">
-        <f>IF(ISNUMBER(Mask!I15),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J15" t="str">
-        <f>IF(ISNUMBER(Mask!J15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="K15" t="str">
-        <f>IF(ISNUMBER(Mask!K15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="L15" t="str">
-        <f>IF(ISNUMBER(Mask!L15),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M15" t="str">
-        <f>IF(ISNUMBER(Mask!M15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="N15" t="str">
-        <f>IF(ISNUMBER(Mask!N15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="O15" t="str">
-        <f>IF(ISNUMBER(Mask!O15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="P15" t="str">
-        <f>IF(ISNUMBER(Mask!P15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="Q15" t="str">
-        <f>IF(ISNUMBER(Mask!Q15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="R15" t="str">
-        <f>IF(ISNUMBER(Mask!R15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" t="s">
+        <v>3</v>
+      </c>
+      <c r="L15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>3</v>
+      </c>
+      <c r="N15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>3</v>
+      </c>
+      <c r="R15" t="s">
+        <v>3</v>
       </c>
       <c r="T15" t="s">
         <v>1</v>
@@ -3644,73 +3443,56 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="str">
-        <f>IF(ISNUMBER(Mask!B16),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C16" t="str">
-        <f>IF(ISNUMBER(Mask!C16),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D16" t="str">
-        <f>IF(ISNUMBER(Mask!D16),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E16" t="str">
-        <f>IF(ISNUMBER(Mask!E16),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F16" t="str">
-        <f>IF(ISNUMBER(Mask!F16),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G16" t="str">
-        <f>IF(ISNUMBER(Mask!G16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="H16" t="str">
-        <f>IF(ISNUMBER(Mask!H16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="I16" t="str">
-        <f>IF(ISNUMBER(Mask!I16),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J16" t="str">
-        <f>IF(ISNUMBER(Mask!J16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="K16" t="str">
-        <f>IF(ISNUMBER(Mask!K16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="L16" t="str">
-        <f>IF(ISNUMBER(Mask!L16),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M16" t="str">
-        <f>IF(ISNUMBER(Mask!M16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="N16" t="str">
-        <f>IF(ISNUMBER(Mask!N16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="O16" t="str">
-        <f>IF(ISNUMBER(Mask!O16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="P16" t="str">
-        <f>IF(ISNUMBER(Mask!P16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="Q16" t="str">
-        <f>IF(ISNUMBER(Mask!Q16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="R16" t="str">
-        <f>IF(ISNUMBER(Mask!R16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K16" t="s">
+        <v>6</v>
+      </c>
+      <c r="L16" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" t="s">
+        <v>3</v>
+      </c>
+      <c r="P16" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>3</v>
+      </c>
+      <c r="R16" t="s">
+        <v>3</v>
       </c>
       <c r="T16" t="s">
         <v>1</v>
@@ -3723,73 +3505,56 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="str">
-        <f>IF(ISNUMBER(Mask!B17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C17" t="str">
-        <f>IF(ISNUMBER(Mask!C17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D17" t="str">
-        <f>IF(ISNUMBER(Mask!D17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E17" t="str">
-        <f>IF(ISNUMBER(Mask!E17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F17" t="str">
-        <f>IF(ISNUMBER(Mask!F17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G17" t="str">
-        <f>IF(ISNUMBER(Mask!G17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="H17" t="str">
-        <f>IF(ISNUMBER(Mask!H17),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="I17" t="str">
-        <f>IF(ISNUMBER(Mask!I17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J17" t="str">
-        <f>IF(ISNUMBER(Mask!J17),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="K17" t="str">
-        <f>IF(ISNUMBER(Mask!K17),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="L17" t="str">
-        <f>IF(ISNUMBER(Mask!L17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M17" t="str">
-        <f>IF(ISNUMBER(Mask!M17),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="N17" t="str">
-        <f>IF(ISNUMBER(Mask!N17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="O17" t="str">
-        <f>IF(ISNUMBER(Mask!O17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="P17" t="str">
-        <f>IF(ISNUMBER(Mask!P17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q17" t="str">
-        <f>IF(ISNUMBER(Mask!Q17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R17" t="str">
-        <f>IF(ISNUMBER(Mask!R17),setup!$F$1,"")</f>
-        <v/>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" t="s">
+        <v>3</v>
+      </c>
+      <c r="N17" t="s">
+        <v>1</v>
+      </c>
+      <c r="O17" t="s">
+        <v>1</v>
+      </c>
+      <c r="P17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" t="s">
+        <v>1</v>
       </c>
       <c r="T17" t="s">
         <v>1</v>
@@ -3802,73 +3567,56 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="str">
-        <f>IF(ISNUMBER(Mask!B18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C18" t="str">
-        <f>IF(ISNUMBER(Mask!C18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D18" t="str">
-        <f>IF(ISNUMBER(Mask!D18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E18" t="str">
-        <f>IF(ISNUMBER(Mask!E18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F18" t="str">
-        <f>IF(ISNUMBER(Mask!F18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G18" t="str">
-        <f>IF(ISNUMBER(Mask!G18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="H18" t="str">
-        <f>IF(ISNUMBER(Mask!H18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="I18" t="str">
-        <f>IF(ISNUMBER(Mask!I18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J18" t="str">
-        <f>IF(ISNUMBER(Mask!J18),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="K18" t="str">
-        <f>IF(ISNUMBER(Mask!K18),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="L18" t="str">
-        <f>IF(ISNUMBER(Mask!L18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M18" t="str">
-        <f>IF(ISNUMBER(Mask!M18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="N18" t="str">
-        <f>IF(ISNUMBER(Mask!N18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="O18" t="str">
-        <f>IF(ISNUMBER(Mask!O18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="P18" t="str">
-        <f>IF(ISNUMBER(Mask!P18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q18" t="str">
-        <f>IF(ISNUMBER(Mask!Q18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R18" t="str">
-        <f>IF(ISNUMBER(Mask!R18),setup!$F$1,"")</f>
-        <v/>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" t="s">
+        <v>3</v>
+      </c>
+      <c r="L18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M18" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18" t="s">
+        <v>1</v>
+      </c>
+      <c r="O18" t="s">
+        <v>1</v>
+      </c>
+      <c r="P18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" t="s">
+        <v>1</v>
       </c>
       <c r="T18" t="s">
         <v>1</v>
@@ -3881,73 +3629,56 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="str">
-        <f>IF(ISNUMBER(Mask!B19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C19" t="str">
-        <f>IF(ISNUMBER(Mask!C19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D19" t="str">
-        <f>IF(ISNUMBER(Mask!D19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E19" t="str">
-        <f>IF(ISNUMBER(Mask!E19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F19" t="str">
-        <f>IF(ISNUMBER(Mask!F19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G19" t="str">
-        <f>IF(ISNUMBER(Mask!G19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="H19" t="str">
-        <f>IF(ISNUMBER(Mask!H19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="I19" t="str">
-        <f>IF(ISNUMBER(Mask!I19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J19" t="str">
-        <f>IF(ISNUMBER(Mask!J19),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="K19" t="str">
-        <f>IF(ISNUMBER(Mask!K19),setup!$F$1,"")</f>
-        <v>100,100,100</v>
-      </c>
-      <c r="L19" t="str">
-        <f>IF(ISNUMBER(Mask!L19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M19" t="str">
-        <f>IF(ISNUMBER(Mask!M19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="N19" t="str">
-        <f>IF(ISNUMBER(Mask!N19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="O19" t="str">
-        <f>IF(ISNUMBER(Mask!O19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="P19" t="str">
-        <f>IF(ISNUMBER(Mask!P19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q19" t="str">
-        <f>IF(ISNUMBER(Mask!Q19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R19" t="str">
-        <f>IF(ISNUMBER(Mask!R19),setup!$F$1,"")</f>
-        <v/>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K19" t="s">
+        <v>3</v>
+      </c>
+      <c r="L19" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" t="s">
+        <v>1</v>
+      </c>
+      <c r="O19" t="s">
+        <v>1</v>
+      </c>
+      <c r="P19" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" t="s">
+        <v>1</v>
       </c>
       <c r="T19" t="s">
         <v>1</v>
@@ -4042,8 +3773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF6F8B5-AF9A-4C54-8212-EFBD25DA246B}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4280,7 +4011,7 @@
       </c>
       <c r="H4" t="str">
         <f>IF(ISNUMBER(Mask!H4),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I4" t="str">
         <f>IF(ISNUMBER(Mask!I4),setup!$F$1,"")</f>
@@ -4288,19 +4019,19 @@
       </c>
       <c r="J4" t="str">
         <f>IF(ISNUMBER(Mask!J4),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K4" t="str">
         <f>IF(ISNUMBER(Mask!K4),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L4" t="str">
         <f>IF(ISNUMBER(Mask!L4),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="M4" t="str">
         <f>IF(ISNUMBER(Mask!M4),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N4" t="str">
         <f>IF(ISNUMBER(Mask!N4),setup!$F$1,"")</f>
@@ -4341,47 +4072,47 @@
       </c>
       <c r="E5" t="str">
         <f>IF(ISNUMBER(Mask!E5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F5" t="str">
         <f>IF(ISNUMBER(Mask!F5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G5" t="str">
         <f>IF(ISNUMBER(Mask!G5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H5" t="str">
         <f>IF(ISNUMBER(Mask!H5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I5" t="str">
         <f>IF(ISNUMBER(Mask!I5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="J5" t="str">
         <f>IF(ISNUMBER(Mask!J5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K5" t="str">
         <f>IF(ISNUMBER(Mask!K5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L5" t="str">
         <f>IF(ISNUMBER(Mask!L5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="M5" t="str">
         <f>IF(ISNUMBER(Mask!M5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N5" t="str">
         <f>IF(ISNUMBER(Mask!N5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O5" t="str">
         <f>IF(ISNUMBER(Mask!O5),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P5" t="str">
         <f>IF(ISNUMBER(Mask!P5),setup!$F$1,"")</f>
@@ -4410,55 +4141,55 @@
       </c>
       <c r="D6" t="str">
         <f>IF(ISNUMBER(Mask!D6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E6" t="str">
         <f>IF(ISNUMBER(Mask!E6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F6" t="str">
         <f>IF(ISNUMBER(Mask!F6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G6" t="str">
         <f>IF(ISNUMBER(Mask!G6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H6" t="str">
         <f>IF(ISNUMBER(Mask!H6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I6" t="str">
         <f>IF(ISNUMBER(Mask!I6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="J6" t="str">
         <f>IF(ISNUMBER(Mask!J6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K6" t="str">
         <f>IF(ISNUMBER(Mask!K6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L6" t="str">
         <f>IF(ISNUMBER(Mask!L6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="M6" t="str">
         <f>IF(ISNUMBER(Mask!M6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N6" t="str">
         <f>IF(ISNUMBER(Mask!N6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O6" t="str">
         <f>IF(ISNUMBER(Mask!O6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P6" t="str">
         <f>IF(ISNUMBER(Mask!P6),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q6" t="str">
         <f>IF(ISNUMBER(Mask!Q6),setup!$F$1,"")</f>
@@ -4479,63 +4210,63 @@
       </c>
       <c r="C7" t="str">
         <f>IF(ISNUMBER(Mask!C7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D7" t="str">
         <f>IF(ISNUMBER(Mask!D7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E7" t="str">
         <f>IF(ISNUMBER(Mask!E7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F7" t="str">
         <f>IF(ISNUMBER(Mask!F7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G7" t="str">
         <f>IF(ISNUMBER(Mask!G7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H7" t="str">
         <f>IF(ISNUMBER(Mask!H7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I7" t="str">
         <f>IF(ISNUMBER(Mask!I7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="J7" t="str">
         <f>IF(ISNUMBER(Mask!J7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K7" t="str">
         <f>IF(ISNUMBER(Mask!K7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L7" t="str">
         <f>IF(ISNUMBER(Mask!L7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="M7" t="str">
         <f>IF(ISNUMBER(Mask!M7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N7" t="str">
         <f>IF(ISNUMBER(Mask!N7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O7" t="str">
         <f>IF(ISNUMBER(Mask!O7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P7" t="str">
         <f>IF(ISNUMBER(Mask!P7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q7" t="str">
         <f>IF(ISNUMBER(Mask!Q7),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R7" t="str">
         <f>IF(ISNUMBER(Mask!R7),setup!$F$1,"")</f>
@@ -4552,63 +4283,63 @@
       </c>
       <c r="C8" t="str">
         <f>IF(ISNUMBER(Mask!C8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D8" t="str">
         <f>IF(ISNUMBER(Mask!D8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E8" t="str">
         <f>IF(ISNUMBER(Mask!E8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F8" t="str">
         <f>IF(ISNUMBER(Mask!F8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G8" t="str">
         <f>IF(ISNUMBER(Mask!G8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H8" t="str">
         <f>IF(ISNUMBER(Mask!H8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I8" t="str">
         <f>IF(ISNUMBER(Mask!I8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="J8" t="str">
         <f>IF(ISNUMBER(Mask!J8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K8" t="str">
         <f>IF(ISNUMBER(Mask!K8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L8" t="str">
         <f>IF(ISNUMBER(Mask!L8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="M8" t="str">
         <f>IF(ISNUMBER(Mask!M8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N8" t="str">
         <f>IF(ISNUMBER(Mask!N8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O8" t="str">
         <f>IF(ISNUMBER(Mask!O8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P8" t="str">
         <f>IF(ISNUMBER(Mask!P8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q8" t="str">
         <f>IF(ISNUMBER(Mask!Q8),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R8" t="str">
         <f>IF(ISNUMBER(Mask!R8),setup!$F$1,"")</f>
@@ -4625,67 +4356,67 @@
       </c>
       <c r="C9" t="str">
         <f>IF(ISNUMBER(Mask!C9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D9" t="str">
         <f>IF(ISNUMBER(Mask!D9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E9" t="str">
         <f>IF(ISNUMBER(Mask!E9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F9" t="str">
         <f>IF(ISNUMBER(Mask!F9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G9" t="str">
         <f>IF(ISNUMBER(Mask!G9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H9" t="str">
         <f>IF(ISNUMBER(Mask!H9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I9" t="str">
         <f>IF(ISNUMBER(Mask!I9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="J9" t="str">
         <f>IF(ISNUMBER(Mask!J9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K9" t="str">
         <f>IF(ISNUMBER(Mask!K9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L9" t="str">
         <f>IF(ISNUMBER(Mask!L9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="M9" t="str">
         <f>IF(ISNUMBER(Mask!M9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N9" t="str">
         <f>IF(ISNUMBER(Mask!N9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O9" t="str">
         <f>IF(ISNUMBER(Mask!O9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P9" t="str">
         <f>IF(ISNUMBER(Mask!P9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q9" t="str">
         <f>IF(ISNUMBER(Mask!Q9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R9" t="str">
         <f>IF(ISNUMBER(Mask!R9),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
@@ -4698,67 +4429,67 @@
       </c>
       <c r="C10" t="str">
         <f>IF(ISNUMBER(Mask!C10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D10" t="str">
         <f>IF(ISNUMBER(Mask!D10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E10" t="str">
         <f>IF(ISNUMBER(Mask!E10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F10" t="str">
         <f>IF(ISNUMBER(Mask!F10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G10" t="str">
         <f>IF(ISNUMBER(Mask!G10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H10" t="str">
         <f>IF(ISNUMBER(Mask!H10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I10" t="str">
         <f>IF(ISNUMBER(Mask!I10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="J10" t="str">
         <f>IF(ISNUMBER(Mask!J10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K10" t="str">
         <f>IF(ISNUMBER(Mask!K10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L10" t="str">
         <f>IF(ISNUMBER(Mask!L10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="M10" t="str">
         <f>IF(ISNUMBER(Mask!M10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N10" t="str">
         <f>IF(ISNUMBER(Mask!N10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O10" t="str">
         <f>IF(ISNUMBER(Mask!O10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P10" t="str">
         <f>IF(ISNUMBER(Mask!P10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q10" t="str">
         <f>IF(ISNUMBER(Mask!Q10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R10" t="str">
         <f>IF(ISNUMBER(Mask!R10),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
@@ -4771,7 +4502,7 @@
       </c>
       <c r="C11" t="str">
         <f>IF(ISNUMBER(Mask!C11),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D11" t="str">
         <f>IF(ISNUMBER(Mask!D11),setup!$F$1,"")</f>
@@ -4844,27 +4575,27 @@
       </c>
       <c r="C12" t="str">
         <f>IF(ISNUMBER(Mask!C12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D12" t="str">
         <f>IF(ISNUMBER(Mask!D12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E12" t="str">
         <f>IF(ISNUMBER(Mask!E12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F12" t="str">
         <f>IF(ISNUMBER(Mask!F12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G12" t="str">
         <f>IF(ISNUMBER(Mask!G12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H12" t="str">
         <f>IF(ISNUMBER(Mask!H12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I12" t="str">
         <f>IF(ISNUMBER(Mask!I12),setup!$F$1,"")</f>
@@ -4872,11 +4603,11 @@
       </c>
       <c r="J12" t="str">
         <f>IF(ISNUMBER(Mask!J12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K12" t="str">
         <f>IF(ISNUMBER(Mask!K12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L12" t="str">
         <f>IF(ISNUMBER(Mask!L12),setup!$F$1,"")</f>
@@ -4884,27 +4615,27 @@
       </c>
       <c r="M12" t="str">
         <f>IF(ISNUMBER(Mask!M12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N12" t="str">
         <f>IF(ISNUMBER(Mask!N12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O12" t="str">
         <f>IF(ISNUMBER(Mask!O12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P12" t="str">
         <f>IF(ISNUMBER(Mask!P12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q12" t="str">
         <f>IF(ISNUMBER(Mask!Q12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R12" t="str">
         <f>IF(ISNUMBER(Mask!R12),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
@@ -4917,27 +4648,27 @@
       </c>
       <c r="C13" t="str">
         <f>IF(ISNUMBER(Mask!C13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D13" t="str">
         <f>IF(ISNUMBER(Mask!D13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E13" t="str">
         <f>IF(ISNUMBER(Mask!E13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F13" t="str">
         <f>IF(ISNUMBER(Mask!F13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G13" t="str">
         <f>IF(ISNUMBER(Mask!G13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H13" t="str">
         <f>IF(ISNUMBER(Mask!H13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I13" t="str">
         <f>IF(ISNUMBER(Mask!I13),setup!$F$1,"")</f>
@@ -4945,11 +4676,11 @@
       </c>
       <c r="J13" t="str">
         <f>IF(ISNUMBER(Mask!J13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K13" t="str">
         <f>IF(ISNUMBER(Mask!K13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L13" t="str">
         <f>IF(ISNUMBER(Mask!L13),setup!$F$1,"")</f>
@@ -4957,27 +4688,27 @@
       </c>
       <c r="M13" t="str">
         <f>IF(ISNUMBER(Mask!M13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N13" t="str">
         <f>IF(ISNUMBER(Mask!N13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O13" t="str">
         <f>IF(ISNUMBER(Mask!O13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P13" t="str">
         <f>IF(ISNUMBER(Mask!P13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q13" t="str">
         <f>IF(ISNUMBER(Mask!Q13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R13" t="str">
         <f>IF(ISNUMBER(Mask!R13),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
@@ -4990,27 +4721,27 @@
       </c>
       <c r="C14" t="str">
         <f>IF(ISNUMBER(Mask!C14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D14" t="str">
         <f>IF(ISNUMBER(Mask!D14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E14" t="str">
         <f>IF(ISNUMBER(Mask!E14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F14" t="str">
         <f>IF(ISNUMBER(Mask!F14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G14" t="str">
         <f>IF(ISNUMBER(Mask!G14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H14" t="str">
         <f>IF(ISNUMBER(Mask!H14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I14" t="str">
         <f>IF(ISNUMBER(Mask!I14),setup!$F$1,"")</f>
@@ -5018,11 +4749,11 @@
       </c>
       <c r="J14" t="str">
         <f>IF(ISNUMBER(Mask!J14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K14" t="str">
         <f>IF(ISNUMBER(Mask!K14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L14" t="str">
         <f>IF(ISNUMBER(Mask!L14),setup!$F$1,"")</f>
@@ -5030,27 +4761,27 @@
       </c>
       <c r="M14" t="str">
         <f>IF(ISNUMBER(Mask!M14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N14" t="str">
         <f>IF(ISNUMBER(Mask!N14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O14" t="str">
         <f>IF(ISNUMBER(Mask!O14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P14" t="str">
         <f>IF(ISNUMBER(Mask!P14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q14" t="str">
         <f>IF(ISNUMBER(Mask!Q14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R14" t="str">
         <f>IF(ISNUMBER(Mask!R14),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
@@ -5063,27 +4794,27 @@
       </c>
       <c r="C15" t="str">
         <f>IF(ISNUMBER(Mask!C15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="D15" t="str">
         <f>IF(ISNUMBER(Mask!D15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="E15" t="str">
         <f>IF(ISNUMBER(Mask!E15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="F15" t="str">
         <f>IF(ISNUMBER(Mask!F15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="G15" t="str">
         <f>IF(ISNUMBER(Mask!G15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H15" t="str">
         <f>IF(ISNUMBER(Mask!H15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I15" t="str">
         <f>IF(ISNUMBER(Mask!I15),setup!$F$1,"")</f>
@@ -5091,11 +4822,11 @@
       </c>
       <c r="J15" t="str">
         <f>IF(ISNUMBER(Mask!J15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K15" t="str">
         <f>IF(ISNUMBER(Mask!K15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L15" t="str">
         <f>IF(ISNUMBER(Mask!L15),setup!$F$1,"")</f>
@@ -5103,27 +4834,27 @@
       </c>
       <c r="M15" t="str">
         <f>IF(ISNUMBER(Mask!M15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N15" t="str">
         <f>IF(ISNUMBER(Mask!N15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O15" t="str">
         <f>IF(ISNUMBER(Mask!O15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P15" t="str">
         <f>IF(ISNUMBER(Mask!P15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q15" t="str">
         <f>IF(ISNUMBER(Mask!Q15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R15" t="str">
         <f>IF(ISNUMBER(Mask!R15),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
@@ -5152,11 +4883,11 @@
       </c>
       <c r="G16" t="str">
         <f>IF(ISNUMBER(Mask!G16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="H16" t="str">
         <f>IF(ISNUMBER(Mask!H16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I16" t="str">
         <f>IF(ISNUMBER(Mask!I16),setup!$F$1,"")</f>
@@ -5164,11 +4895,11 @@
       </c>
       <c r="J16" t="str">
         <f>IF(ISNUMBER(Mask!J16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K16" t="str">
         <f>IF(ISNUMBER(Mask!K16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L16" t="str">
         <f>IF(ISNUMBER(Mask!L16),setup!$F$1,"")</f>
@@ -5176,27 +4907,27 @@
       </c>
       <c r="M16" t="str">
         <f>IF(ISNUMBER(Mask!M16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N16" t="str">
         <f>IF(ISNUMBER(Mask!N16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="O16" t="str">
         <f>IF(ISNUMBER(Mask!O16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="P16" t="str">
         <f>IF(ISNUMBER(Mask!P16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="Q16" t="str">
         <f>IF(ISNUMBER(Mask!Q16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="R16" t="str">
         <f>IF(ISNUMBER(Mask!R16),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
@@ -5229,7 +4960,7 @@
       </c>
       <c r="H17" t="str">
         <f>IF(ISNUMBER(Mask!H17),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="I17" t="str">
         <f>IF(ISNUMBER(Mask!I17),setup!$F$1,"")</f>
@@ -5237,11 +4968,11 @@
       </c>
       <c r="J17" t="str">
         <f>IF(ISNUMBER(Mask!J17),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K17" t="str">
         <f>IF(ISNUMBER(Mask!K17),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L17" t="str">
         <f>IF(ISNUMBER(Mask!L17),setup!$F$1,"")</f>
@@ -5249,7 +4980,7 @@
       </c>
       <c r="M17" t="str">
         <f>IF(ISNUMBER(Mask!M17),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="N17" t="str">
         <f>IF(ISNUMBER(Mask!N17),setup!$F$1,"")</f>
@@ -5310,11 +5041,11 @@
       </c>
       <c r="J18" t="str">
         <f>IF(ISNUMBER(Mask!J18),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K18" t="str">
         <f>IF(ISNUMBER(Mask!K18),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L18" t="str">
         <f>IF(ISNUMBER(Mask!L18),setup!$F$1,"")</f>
@@ -5383,11 +5114,11 @@
       </c>
       <c r="J19" t="str">
         <f>IF(ISNUMBER(Mask!J19),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="K19" t="str">
         <f>IF(ISNUMBER(Mask!K19),setup!$F$1,"")</f>
-        <v>100,100,100</v>
+        <v>138,3,3</v>
       </c>
       <c r="L19" t="str">
         <f>IF(ISNUMBER(Mask!L19),setup!$F$1,"")</f>

</xml_diff>

<commit_message>
testing out the multi array
</commit_message>
<xml_diff>
--- a/blinka/data/grid.xlsx
+++ b/blinka/data/grid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\william.harding\Documents\repos\raspberrypi\blinka\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC9106B-EFF6-4C61-B37A-CC310D349179}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C3B894-EB59-40DF-A967-EE9430D0C41A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="setup" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="8">
   <si>
     <t>default color</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>255,204,0</t>
+  </si>
+  <si>
+    <t>50,0,22</t>
   </si>
 </sst>
 </file>
@@ -2503,8 +2506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C3361C-1C15-4A97-8B76-564436F68EDA}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I11" sqref="A1:U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3771,15 +3774,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF6F8B5-AF9A-4C54-8212-EFBD25DA246B}">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>1</v>
       </c>
@@ -3834,1324 +3837,1203 @@
       <c r="S1">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="T1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="H2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="I2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="K2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="L2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="N2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="O2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="P2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R2" t="str">
-        <f>IF(ISNUMBER(Mask!#REF!),setup!$F$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="str">
-        <f>IF(ISNUMBER(Mask!B3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C3" t="str">
-        <f>IF(ISNUMBER(Mask!C3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D3" t="str">
-        <f>IF(ISNUMBER(Mask!D3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E3" t="str">
-        <f>IF(ISNUMBER(Mask!E3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F3" t="str">
-        <f>IF(ISNUMBER(Mask!F3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G3" t="str">
-        <f>IF(ISNUMBER(Mask!G3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="H3" t="str">
-        <f>IF(ISNUMBER(Mask!H3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="I3" t="str">
-        <f>IF(ISNUMBER(Mask!I3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J3" t="str">
-        <f>IF(ISNUMBER(Mask!J3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="K3" t="str">
-        <f>IF(ISNUMBER(Mask!K3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="L3" t="str">
-        <f>IF(ISNUMBER(Mask!L3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M3" t="str">
-        <f>IF(ISNUMBER(Mask!M3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="N3" t="str">
-        <f>IF(ISNUMBER(Mask!N3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="O3" t="str">
-        <f>IF(ISNUMBER(Mask!O3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="P3" t="str">
-        <f>IF(ISNUMBER(Mask!P3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q3" t="str">
-        <f>IF(ISNUMBER(Mask!Q3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R3" t="str">
-        <f>IF(ISNUMBER(Mask!R3),setup!$F$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="str">
-        <f>IF(ISNUMBER(Mask!B4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C4" t="str">
-        <f>IF(ISNUMBER(Mask!C4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D4" t="str">
-        <f>IF(ISNUMBER(Mask!D4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E4" t="str">
-        <f>IF(ISNUMBER(Mask!E4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F4" t="str">
-        <f>IF(ISNUMBER(Mask!F4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G4" t="str">
-        <f>IF(ISNUMBER(Mask!G4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="H4" t="str">
-        <f>IF(ISNUMBER(Mask!H4),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="I4" t="str">
-        <f>IF(ISNUMBER(Mask!I4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J4" t="str">
-        <f>IF(ISNUMBER(Mask!J4),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="K4" t="str">
-        <f>IF(ISNUMBER(Mask!K4),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="L4" t="str">
-        <f>IF(ISNUMBER(Mask!L4),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="M4" t="str">
-        <f>IF(ISNUMBER(Mask!M4),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="N4" t="str">
-        <f>IF(ISNUMBER(Mask!N4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="O4" t="str">
-        <f>IF(ISNUMBER(Mask!O4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="P4" t="str">
-        <f>IF(ISNUMBER(Mask!P4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q4" t="str">
-        <f>IF(ISNUMBER(Mask!Q4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R4" t="str">
-        <f>IF(ISNUMBER(Mask!R4),setup!$F$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="str">
-        <f>IF(ISNUMBER(Mask!B5),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C5" t="str">
-        <f>IF(ISNUMBER(Mask!C5),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D5" t="str">
-        <f>IF(ISNUMBER(Mask!D5),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E5" t="str">
-        <f>IF(ISNUMBER(Mask!E5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="F5" t="str">
-        <f>IF(ISNUMBER(Mask!F5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="G5" t="str">
-        <f>IF(ISNUMBER(Mask!G5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="H5" t="str">
-        <f>IF(ISNUMBER(Mask!H5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="I5" t="str">
-        <f>IF(ISNUMBER(Mask!I5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="J5" t="str">
-        <f>IF(ISNUMBER(Mask!J5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="K5" t="str">
-        <f>IF(ISNUMBER(Mask!K5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="L5" t="str">
-        <f>IF(ISNUMBER(Mask!L5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="M5" t="str">
-        <f>IF(ISNUMBER(Mask!M5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="N5" t="str">
-        <f>IF(ISNUMBER(Mask!N5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="O5" t="str">
-        <f>IF(ISNUMBER(Mask!O5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="P5" t="str">
-        <f>IF(ISNUMBER(Mask!P5),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q5" t="str">
-        <f>IF(ISNUMBER(Mask!Q5),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R5" t="str">
-        <f>IF(ISNUMBER(Mask!R5),setup!$F$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="str">
-        <f>IF(ISNUMBER(Mask!B6),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C6" t="str">
-        <f>IF(ISNUMBER(Mask!C6),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D6" t="str">
-        <f>IF(ISNUMBER(Mask!D6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="E6" t="str">
-        <f>IF(ISNUMBER(Mask!E6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="F6" t="str">
-        <f>IF(ISNUMBER(Mask!F6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="G6" t="str">
-        <f>IF(ISNUMBER(Mask!G6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="H6" t="str">
-        <f>IF(ISNUMBER(Mask!H6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="I6" t="str">
-        <f>IF(ISNUMBER(Mask!I6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="J6" t="str">
-        <f>IF(ISNUMBER(Mask!J6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="K6" t="str">
-        <f>IF(ISNUMBER(Mask!K6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="L6" t="str">
-        <f>IF(ISNUMBER(Mask!L6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="M6" t="str">
-        <f>IF(ISNUMBER(Mask!M6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="N6" t="str">
-        <f>IF(ISNUMBER(Mask!N6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="O6" t="str">
-        <f>IF(ISNUMBER(Mask!O6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="P6" t="str">
-        <f>IF(ISNUMBER(Mask!P6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="Q6" t="str">
-        <f>IF(ISNUMBER(Mask!Q6),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R6" t="str">
-        <f>IF(ISNUMBER(Mask!R6),setup!$F$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1</v>
+      </c>
+      <c r="T6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="str">
-        <f>IF(ISNUMBER(Mask!B7),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C7" t="str">
-        <f>IF(ISNUMBER(Mask!C7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="D7" t="str">
-        <f>IF(ISNUMBER(Mask!D7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="E7" t="str">
-        <f>IF(ISNUMBER(Mask!E7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="F7" t="str">
-        <f>IF(ISNUMBER(Mask!F7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="G7" t="str">
-        <f>IF(ISNUMBER(Mask!G7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="H7" t="str">
-        <f>IF(ISNUMBER(Mask!H7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="I7" t="str">
-        <f>IF(ISNUMBER(Mask!I7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="J7" t="str">
-        <f>IF(ISNUMBER(Mask!J7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="K7" t="str">
-        <f>IF(ISNUMBER(Mask!K7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="L7" t="str">
-        <f>IF(ISNUMBER(Mask!L7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="M7" t="str">
-        <f>IF(ISNUMBER(Mask!M7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="N7" t="str">
-        <f>IF(ISNUMBER(Mask!N7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="O7" t="str">
-        <f>IF(ISNUMBER(Mask!O7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="P7" t="str">
-        <f>IF(ISNUMBER(Mask!P7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="Q7" t="str">
-        <f>IF(ISNUMBER(Mask!Q7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="R7" t="str">
-        <f>IF(ISNUMBER(Mask!R7),setup!$F$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>3</v>
+      </c>
+      <c r="R7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T7" t="s">
+        <v>1</v>
+      </c>
+      <c r="U7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="str">
-        <f>IF(ISNUMBER(Mask!B8),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C8" t="str">
-        <f>IF(ISNUMBER(Mask!C8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="D8" t="str">
-        <f>IF(ISNUMBER(Mask!D8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="E8" t="str">
-        <f>IF(ISNUMBER(Mask!E8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="F8" t="str">
-        <f>IF(ISNUMBER(Mask!F8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="G8" t="str">
-        <f>IF(ISNUMBER(Mask!G8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="H8" t="str">
-        <f>IF(ISNUMBER(Mask!H8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="I8" t="str">
-        <f>IF(ISNUMBER(Mask!I8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="J8" t="str">
-        <f>IF(ISNUMBER(Mask!J8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="K8" t="str">
-        <f>IF(ISNUMBER(Mask!K8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="L8" t="str">
-        <f>IF(ISNUMBER(Mask!L8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="M8" t="str">
-        <f>IF(ISNUMBER(Mask!M8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="N8" t="str">
-        <f>IF(ISNUMBER(Mask!N8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="O8" t="str">
-        <f>IF(ISNUMBER(Mask!O8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="P8" t="str">
-        <f>IF(ISNUMBER(Mask!P8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="Q8" t="str">
-        <f>IF(ISNUMBER(Mask!Q8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="R8" t="str">
-        <f>IF(ISNUMBER(Mask!R8),setup!$F$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R8" t="s">
+        <v>1</v>
+      </c>
+      <c r="T8" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="str">
-        <f>IF(ISNUMBER(Mask!B9),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C9" t="str">
-        <f>IF(ISNUMBER(Mask!C9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="D9" t="str">
-        <f>IF(ISNUMBER(Mask!D9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="E9" t="str">
-        <f>IF(ISNUMBER(Mask!E9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="F9" t="str">
-        <f>IF(ISNUMBER(Mask!F9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="G9" t="str">
-        <f>IF(ISNUMBER(Mask!G9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="H9" t="str">
-        <f>IF(ISNUMBER(Mask!H9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="I9" t="str">
-        <f>IF(ISNUMBER(Mask!I9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="J9" t="str">
-        <f>IF(ISNUMBER(Mask!J9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="K9" t="str">
-        <f>IF(ISNUMBER(Mask!K9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="L9" t="str">
-        <f>IF(ISNUMBER(Mask!L9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="M9" t="str">
-        <f>IF(ISNUMBER(Mask!M9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="N9" t="str">
-        <f>IF(ISNUMBER(Mask!N9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="O9" t="str">
-        <f>IF(ISNUMBER(Mask!O9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="P9" t="str">
-        <f>IF(ISNUMBER(Mask!P9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="Q9" t="str">
-        <f>IF(ISNUMBER(Mask!Q9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="R9" t="str">
-        <f>IF(ISNUMBER(Mask!R9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>3</v>
+      </c>
+      <c r="R9" t="s">
+        <v>3</v>
+      </c>
+      <c r="T9" t="s">
+        <v>1</v>
+      </c>
+      <c r="U9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="str">
-        <f>IF(ISNUMBER(Mask!B10),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C10" t="str">
-        <f>IF(ISNUMBER(Mask!C10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="D10" t="str">
-        <f>IF(ISNUMBER(Mask!D10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="E10" t="str">
-        <f>IF(ISNUMBER(Mask!E10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="F10" t="str">
-        <f>IF(ISNUMBER(Mask!F10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="G10" t="str">
-        <f>IF(ISNUMBER(Mask!G10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="H10" t="str">
-        <f>IF(ISNUMBER(Mask!H10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="I10" t="str">
-        <f>IF(ISNUMBER(Mask!I10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="J10" t="str">
-        <f>IF(ISNUMBER(Mask!J10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="K10" t="str">
-        <f>IF(ISNUMBER(Mask!K10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="L10" t="str">
-        <f>IF(ISNUMBER(Mask!L10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="M10" t="str">
-        <f>IF(ISNUMBER(Mask!M10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="N10" t="str">
-        <f>IF(ISNUMBER(Mask!N10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="O10" t="str">
-        <f>IF(ISNUMBER(Mask!O10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="P10" t="str">
-        <f>IF(ISNUMBER(Mask!P10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="Q10" t="str">
-        <f>IF(ISNUMBER(Mask!Q10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="R10" t="str">
-        <f>IF(ISNUMBER(Mask!R10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" t="s">
+        <v>3</v>
+      </c>
+      <c r="L10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" t="s">
+        <v>7</v>
+      </c>
+      <c r="O10" t="s">
+        <v>7</v>
+      </c>
+      <c r="P10" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>7</v>
+      </c>
+      <c r="R10" t="s">
+        <v>3</v>
+      </c>
+      <c r="T10" t="s">
+        <v>1</v>
+      </c>
+      <c r="U10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="str">
-        <f>IF(ISNUMBER(Mask!B11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C11" t="str">
-        <f>IF(ISNUMBER(Mask!C11),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="D11" t="str">
-        <f>IF(ISNUMBER(Mask!D11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E11" t="str">
-        <f>IF(ISNUMBER(Mask!E11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F11" t="str">
-        <f>IF(ISNUMBER(Mask!F11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G11" t="str">
-        <f>IF(ISNUMBER(Mask!G11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="H11" t="str">
-        <f>IF(ISNUMBER(Mask!H11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="I11" t="str">
-        <f>IF(ISNUMBER(Mask!I11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J11" t="str">
-        <f>IF(ISNUMBER(Mask!J11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="K11" t="str">
-        <f>IF(ISNUMBER(Mask!K11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="L11" t="str">
-        <f>IF(ISNUMBER(Mask!L11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M11" t="str">
-        <f>IF(ISNUMBER(Mask!M11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="N11" t="str">
-        <f>IF(ISNUMBER(Mask!N11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="O11" t="str">
-        <f>IF(ISNUMBER(Mask!O11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="P11" t="str">
-        <f>IF(ISNUMBER(Mask!P11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q11" t="str">
-        <f>IF(ISNUMBER(Mask!Q11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R11" t="str">
-        <f>IF(ISNUMBER(Mask!R11),setup!$F$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>1</v>
+      </c>
+      <c r="R11" t="s">
+        <v>1</v>
+      </c>
+      <c r="T11" t="s">
+        <v>1</v>
+      </c>
+      <c r="U11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="str">
-        <f>IF(ISNUMBER(Mask!B12),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C12" t="str">
-        <f>IF(ISNUMBER(Mask!C12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="D12" t="str">
-        <f>IF(ISNUMBER(Mask!D12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="E12" t="str">
-        <f>IF(ISNUMBER(Mask!E12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="F12" t="str">
-        <f>IF(ISNUMBER(Mask!F12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="G12" t="str">
-        <f>IF(ISNUMBER(Mask!G12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="H12" t="str">
-        <f>IF(ISNUMBER(Mask!H12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="I12" t="str">
-        <f>IF(ISNUMBER(Mask!I12),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J12" t="str">
-        <f>IF(ISNUMBER(Mask!J12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="K12" t="str">
-        <f>IF(ISNUMBER(Mask!K12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="L12" t="str">
-        <f>IF(ISNUMBER(Mask!L12),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M12" t="str">
-        <f>IF(ISNUMBER(Mask!M12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="N12" t="str">
-        <f>IF(ISNUMBER(Mask!N12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="O12" t="str">
-        <f>IF(ISNUMBER(Mask!O12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="P12" t="str">
-        <f>IF(ISNUMBER(Mask!P12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="Q12" t="str">
-        <f>IF(ISNUMBER(Mask!Q12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="R12" t="str">
-        <f>IF(ISNUMBER(Mask!R12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" t="s">
+        <v>3</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12" t="s">
+        <v>7</v>
+      </c>
+      <c r="O12" t="s">
+        <v>7</v>
+      </c>
+      <c r="P12" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>7</v>
+      </c>
+      <c r="R12" t="s">
+        <v>3</v>
+      </c>
+      <c r="T12" t="s">
+        <v>1</v>
+      </c>
+      <c r="U12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="str">
-        <f>IF(ISNUMBER(Mask!B13),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C13" t="str">
-        <f>IF(ISNUMBER(Mask!C13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="D13" t="str">
-        <f>IF(ISNUMBER(Mask!D13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="E13" t="str">
-        <f>IF(ISNUMBER(Mask!E13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="F13" t="str">
-        <f>IF(ISNUMBER(Mask!F13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="G13" t="str">
-        <f>IF(ISNUMBER(Mask!G13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="H13" t="str">
-        <f>IF(ISNUMBER(Mask!H13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="I13" t="str">
-        <f>IF(ISNUMBER(Mask!I13),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J13" t="str">
-        <f>IF(ISNUMBER(Mask!J13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="K13" t="str">
-        <f>IF(ISNUMBER(Mask!K13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="L13" t="str">
-        <f>IF(ISNUMBER(Mask!L13),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M13" t="str">
-        <f>IF(ISNUMBER(Mask!M13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="N13" t="str">
-        <f>IF(ISNUMBER(Mask!N13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="O13" t="str">
-        <f>IF(ISNUMBER(Mask!O13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="P13" t="str">
-        <f>IF(ISNUMBER(Mask!P13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="Q13" t="str">
-        <f>IF(ISNUMBER(Mask!Q13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="R13" t="str">
-        <f>IF(ISNUMBER(Mask!R13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13" t="s">
+        <v>3</v>
+      </c>
+      <c r="O13" t="s">
+        <v>3</v>
+      </c>
+      <c r="P13" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>3</v>
+      </c>
+      <c r="R13" t="s">
+        <v>3</v>
+      </c>
+      <c r="T13" t="s">
+        <v>1</v>
+      </c>
+      <c r="U13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="str">
-        <f>IF(ISNUMBER(Mask!B14),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C14" t="str">
-        <f>IF(ISNUMBER(Mask!C14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="D14" t="str">
-        <f>IF(ISNUMBER(Mask!D14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="E14" t="str">
-        <f>IF(ISNUMBER(Mask!E14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="F14" t="str">
-        <f>IF(ISNUMBER(Mask!F14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="G14" t="str">
-        <f>IF(ISNUMBER(Mask!G14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="H14" t="str">
-        <f>IF(ISNUMBER(Mask!H14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="I14" t="str">
-        <f>IF(ISNUMBER(Mask!I14),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J14" t="str">
-        <f>IF(ISNUMBER(Mask!J14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="K14" t="str">
-        <f>IF(ISNUMBER(Mask!K14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="L14" t="str">
-        <f>IF(ISNUMBER(Mask!L14),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M14" t="str">
-        <f>IF(ISNUMBER(Mask!M14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="N14" t="str">
-        <f>IF(ISNUMBER(Mask!N14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="O14" t="str">
-        <f>IF(ISNUMBER(Mask!O14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="P14" t="str">
-        <f>IF(ISNUMBER(Mask!P14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="Q14" t="str">
-        <f>IF(ISNUMBER(Mask!Q14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="R14" t="str">
-        <f>IF(ISNUMBER(Mask!R14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" t="s">
+        <v>7</v>
+      </c>
+      <c r="N14" t="s">
+        <v>7</v>
+      </c>
+      <c r="O14" t="s">
+        <v>3</v>
+      </c>
+      <c r="P14" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>3</v>
+      </c>
+      <c r="R14" t="s">
+        <v>3</v>
+      </c>
+      <c r="T14" t="s">
+        <v>1</v>
+      </c>
+      <c r="U14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="str">
-        <f>IF(ISNUMBER(Mask!B15),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C15" t="str">
-        <f>IF(ISNUMBER(Mask!C15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="D15" t="str">
-        <f>IF(ISNUMBER(Mask!D15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="E15" t="str">
-        <f>IF(ISNUMBER(Mask!E15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="F15" t="str">
-        <f>IF(ISNUMBER(Mask!F15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="G15" t="str">
-        <f>IF(ISNUMBER(Mask!G15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="H15" t="str">
-        <f>IF(ISNUMBER(Mask!H15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="I15" t="str">
-        <f>IF(ISNUMBER(Mask!I15),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J15" t="str">
-        <f>IF(ISNUMBER(Mask!J15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="K15" t="str">
-        <f>IF(ISNUMBER(Mask!K15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="L15" t="str">
-        <f>IF(ISNUMBER(Mask!L15),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M15" t="str">
-        <f>IF(ISNUMBER(Mask!M15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="N15" t="str">
-        <f>IF(ISNUMBER(Mask!N15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="O15" t="str">
-        <f>IF(ISNUMBER(Mask!O15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="P15" t="str">
-        <f>IF(ISNUMBER(Mask!P15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="Q15" t="str">
-        <f>IF(ISNUMBER(Mask!Q15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="R15" t="str">
-        <f>IF(ISNUMBER(Mask!R15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" t="s">
+        <v>3</v>
+      </c>
+      <c r="L15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>7</v>
+      </c>
+      <c r="N15" t="s">
+        <v>7</v>
+      </c>
+      <c r="O15" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>3</v>
+      </c>
+      <c r="R15" t="s">
+        <v>3</v>
+      </c>
+      <c r="T15" t="s">
+        <v>1</v>
+      </c>
+      <c r="U15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="str">
-        <f>IF(ISNUMBER(Mask!B16),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C16" t="str">
-        <f>IF(ISNUMBER(Mask!C16),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D16" t="str">
-        <f>IF(ISNUMBER(Mask!D16),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E16" t="str">
-        <f>IF(ISNUMBER(Mask!E16),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F16" t="str">
-        <f>IF(ISNUMBER(Mask!F16),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G16" t="str">
-        <f>IF(ISNUMBER(Mask!G16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="H16" t="str">
-        <f>IF(ISNUMBER(Mask!H16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="I16" t="str">
-        <f>IF(ISNUMBER(Mask!I16),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J16" t="str">
-        <f>IF(ISNUMBER(Mask!J16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="K16" t="str">
-        <f>IF(ISNUMBER(Mask!K16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="L16" t="str">
-        <f>IF(ISNUMBER(Mask!L16),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M16" t="str">
-        <f>IF(ISNUMBER(Mask!M16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="N16" t="str">
-        <f>IF(ISNUMBER(Mask!N16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="O16" t="str">
-        <f>IF(ISNUMBER(Mask!O16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="P16" t="str">
-        <f>IF(ISNUMBER(Mask!P16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="Q16" t="str">
-        <f>IF(ISNUMBER(Mask!Q16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="R16" t="str">
-        <f>IF(ISNUMBER(Mask!R16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" t="s">
+        <v>7</v>
+      </c>
+      <c r="L16" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" t="s">
+        <v>3</v>
+      </c>
+      <c r="P16" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>3</v>
+      </c>
+      <c r="R16" t="s">
+        <v>3</v>
+      </c>
+      <c r="T16" t="s">
+        <v>1</v>
+      </c>
+      <c r="U16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="str">
-        <f>IF(ISNUMBER(Mask!B17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C17" t="str">
-        <f>IF(ISNUMBER(Mask!C17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D17" t="str">
-        <f>IF(ISNUMBER(Mask!D17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E17" t="str">
-        <f>IF(ISNUMBER(Mask!E17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F17" t="str">
-        <f>IF(ISNUMBER(Mask!F17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G17" t="str">
-        <f>IF(ISNUMBER(Mask!G17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="H17" t="str">
-        <f>IF(ISNUMBER(Mask!H17),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="I17" t="str">
-        <f>IF(ISNUMBER(Mask!I17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J17" t="str">
-        <f>IF(ISNUMBER(Mask!J17),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="K17" t="str">
-        <f>IF(ISNUMBER(Mask!K17),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="L17" t="str">
-        <f>IF(ISNUMBER(Mask!L17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M17" t="str">
-        <f>IF(ISNUMBER(Mask!M17),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="N17" t="str">
-        <f>IF(ISNUMBER(Mask!N17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="O17" t="str">
-        <f>IF(ISNUMBER(Mask!O17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="P17" t="str">
-        <f>IF(ISNUMBER(Mask!P17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q17" t="str">
-        <f>IF(ISNUMBER(Mask!Q17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R17" t="str">
-        <f>IF(ISNUMBER(Mask!R17),setup!$F$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" t="s">
+        <v>7</v>
+      </c>
+      <c r="L17" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" t="s">
+        <v>3</v>
+      </c>
+      <c r="N17" t="s">
+        <v>1</v>
+      </c>
+      <c r="O17" t="s">
+        <v>1</v>
+      </c>
+      <c r="P17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" t="s">
+        <v>1</v>
+      </c>
+      <c r="T17" t="s">
+        <v>1</v>
+      </c>
+      <c r="U17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="str">
-        <f>IF(ISNUMBER(Mask!B18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C18" t="str">
-        <f>IF(ISNUMBER(Mask!C18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D18" t="str">
-        <f>IF(ISNUMBER(Mask!D18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E18" t="str">
-        <f>IF(ISNUMBER(Mask!E18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F18" t="str">
-        <f>IF(ISNUMBER(Mask!F18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G18" t="str">
-        <f>IF(ISNUMBER(Mask!G18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="H18" t="str">
-        <f>IF(ISNUMBER(Mask!H18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="I18" t="str">
-        <f>IF(ISNUMBER(Mask!I18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J18" t="str">
-        <f>IF(ISNUMBER(Mask!J18),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="K18" t="str">
-        <f>IF(ISNUMBER(Mask!K18),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="L18" t="str">
-        <f>IF(ISNUMBER(Mask!L18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M18" t="str">
-        <f>IF(ISNUMBER(Mask!M18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="N18" t="str">
-        <f>IF(ISNUMBER(Mask!N18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="O18" t="str">
-        <f>IF(ISNUMBER(Mask!O18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="P18" t="str">
-        <f>IF(ISNUMBER(Mask!P18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q18" t="str">
-        <f>IF(ISNUMBER(Mask!Q18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R18" t="str">
-        <f>IF(ISNUMBER(Mask!R18),setup!$F$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" t="s">
+        <v>3</v>
+      </c>
+      <c r="L18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M18" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18" t="s">
+        <v>1</v>
+      </c>
+      <c r="O18" t="s">
+        <v>1</v>
+      </c>
+      <c r="P18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" t="s">
+        <v>1</v>
+      </c>
+      <c r="T18" t="s">
+        <v>1</v>
+      </c>
+      <c r="U18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="str">
-        <f>IF(ISNUMBER(Mask!B19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="C19" t="str">
-        <f>IF(ISNUMBER(Mask!C19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="D19" t="str">
-        <f>IF(ISNUMBER(Mask!D19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="E19" t="str">
-        <f>IF(ISNUMBER(Mask!E19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="F19" t="str">
-        <f>IF(ISNUMBER(Mask!F19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="G19" t="str">
-        <f>IF(ISNUMBER(Mask!G19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="H19" t="str">
-        <f>IF(ISNUMBER(Mask!H19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="I19" t="str">
-        <f>IF(ISNUMBER(Mask!I19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="J19" t="str">
-        <f>IF(ISNUMBER(Mask!J19),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="K19" t="str">
-        <f>IF(ISNUMBER(Mask!K19),setup!$F$1,"")</f>
-        <v>138,3,3</v>
-      </c>
-      <c r="L19" t="str">
-        <f>IF(ISNUMBER(Mask!L19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="M19" t="str">
-        <f>IF(ISNUMBER(Mask!M19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="N19" t="str">
-        <f>IF(ISNUMBER(Mask!N19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="O19" t="str">
-        <f>IF(ISNUMBER(Mask!O19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="P19" t="str">
-        <f>IF(ISNUMBER(Mask!P19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="Q19" t="str">
-        <f>IF(ISNUMBER(Mask!Q19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-      <c r="R19" t="str">
-        <f>IF(ISNUMBER(Mask!R19),setup!$F$1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K19" t="s">
+        <v>3</v>
+      </c>
+      <c r="L19" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" t="s">
+        <v>1</v>
+      </c>
+      <c r="O19" t="s">
+        <v>1</v>
+      </c>
+      <c r="P19" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" t="s">
+        <v>1</v>
+      </c>
+      <c r="T19" t="s">
+        <v>1</v>
+      </c>
+      <c r="U19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
+      </c>
+      <c r="T20" t="s">
+        <v>1</v>
+      </c>
+      <c r="U20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" t="s">
+        <v>1</v>
+      </c>
+      <c r="M21" t="s">
+        <v>1</v>
+      </c>
+      <c r="N21" t="s">
+        <v>1</v>
+      </c>
+      <c r="O21" t="s">
+        <v>1</v>
+      </c>
+      <c r="P21" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>1</v>
+      </c>
+      <c r="R21" t="s">
+        <v>1</v>
+      </c>
+      <c r="S21" t="s">
+        <v>1</v>
+      </c>
+      <c r="T21" t="s">
+        <v>1</v>
+      </c>
+      <c r="U21" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
took out null and added extra pattern
</commit_message>
<xml_diff>
--- a/blinka/data/grid.xlsx
+++ b/blinka/data/grid.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\william.harding\Documents\repos\raspberrypi\blinka\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C3B894-EB59-40DF-A967-EE9430D0C41A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087A5E0F-DECC-4935-9F16-FD479232DF98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="setup" sheetId="3" r:id="rId1"/>
     <sheet name="Mask" sheetId="2" r:id="rId2"/>
     <sheet name="sheetmaker" sheetId="1" r:id="rId3"/>
-    <sheet name="pattern 1" sheetId="4" r:id="rId4"/>
-    <sheet name="pattern 2" sheetId="5" r:id="rId5"/>
+    <sheet name="pattern 3" sheetId="6" r:id="rId4"/>
+    <sheet name="pattern 1" sheetId="4" r:id="rId5"/>
+    <sheet name="pattern 2" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="9">
   <si>
     <t>default color</t>
   </si>
@@ -62,6 +63,9 @@
   </si>
   <si>
     <t>50,0,22</t>
+  </si>
+  <si>
+    <t>0,0,0</t>
   </si>
 </sst>
 </file>
@@ -382,7 +386,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -407,7 +411,7 @@
         <v>100</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1112,7 +1116,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView zoomScale="61" workbookViewId="0">
-      <selection activeCell="F16" sqref="A1:S20"/>
+      <selection activeCell="E16" sqref="A1:S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1353,7 +1357,7 @@
       </c>
       <c r="H4" t="str">
         <f>IF(ISNUMBER(Mask!H4),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="I4" t="str">
         <f>IF(ISNUMBER(Mask!I4),setup!$F$1,"")</f>
@@ -1361,19 +1365,19 @@
       </c>
       <c r="J4" t="str">
         <f>IF(ISNUMBER(Mask!J4),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="K4" t="str">
         <f>IF(ISNUMBER(Mask!K4),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="L4" t="str">
         <f>IF(ISNUMBER(Mask!L4),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="M4" t="str">
         <f>IF(ISNUMBER(Mask!M4),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="N4" t="str">
         <f>IF(ISNUMBER(Mask!N4),setup!$F$1,"")</f>
@@ -1414,47 +1418,47 @@
       </c>
       <c r="E5" t="str">
         <f>IF(ISNUMBER(Mask!E5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="F5" t="str">
         <f>IF(ISNUMBER(Mask!F5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="G5" t="str">
         <f>IF(ISNUMBER(Mask!G5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="H5" t="str">
         <f>IF(ISNUMBER(Mask!H5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="I5" t="str">
         <f>IF(ISNUMBER(Mask!I5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="J5" t="str">
         <f>IF(ISNUMBER(Mask!J5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="K5" t="str">
         <f>IF(ISNUMBER(Mask!K5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="L5" t="str">
         <f>IF(ISNUMBER(Mask!L5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="M5" t="str">
         <f>IF(ISNUMBER(Mask!M5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="N5" t="str">
         <f>IF(ISNUMBER(Mask!N5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="O5" t="str">
         <f>IF(ISNUMBER(Mask!O5),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="P5" t="str">
         <f>IF(ISNUMBER(Mask!P5),setup!$F$1,"")</f>
@@ -1483,55 +1487,55 @@
       </c>
       <c r="D6" t="str">
         <f>IF(ISNUMBER(Mask!D6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="E6" t="str">
         <f>IF(ISNUMBER(Mask!E6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="F6" t="str">
         <f>IF(ISNUMBER(Mask!F6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="G6" t="str">
         <f>IF(ISNUMBER(Mask!G6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="H6" t="str">
         <f>IF(ISNUMBER(Mask!H6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="I6" t="str">
         <f>IF(ISNUMBER(Mask!I6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="J6" t="str">
         <f>IF(ISNUMBER(Mask!J6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="K6" t="str">
         <f>IF(ISNUMBER(Mask!K6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="L6" t="str">
         <f>IF(ISNUMBER(Mask!L6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="M6" t="str">
         <f>IF(ISNUMBER(Mask!M6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="N6" t="str">
         <f>IF(ISNUMBER(Mask!N6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="O6" t="str">
         <f>IF(ISNUMBER(Mask!O6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="P6" t="str">
         <f>IF(ISNUMBER(Mask!P6),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="Q6" t="str">
         <f>IF(ISNUMBER(Mask!Q6),setup!$F$1,"")</f>
@@ -1552,63 +1556,63 @@
       </c>
       <c r="C7" t="str">
         <f>IF(ISNUMBER(Mask!C7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="D7" t="str">
         <f>IF(ISNUMBER(Mask!D7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="E7" t="str">
         <f>IF(ISNUMBER(Mask!E7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="F7" t="str">
         <f>IF(ISNUMBER(Mask!F7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="G7" t="str">
         <f>IF(ISNUMBER(Mask!G7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="H7" t="str">
         <f>IF(ISNUMBER(Mask!H7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="I7" t="str">
         <f>IF(ISNUMBER(Mask!I7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="J7" t="str">
         <f>IF(ISNUMBER(Mask!J7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="K7" t="str">
         <f>IF(ISNUMBER(Mask!K7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="L7" t="str">
         <f>IF(ISNUMBER(Mask!L7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="M7" t="str">
         <f>IF(ISNUMBER(Mask!M7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="N7" t="str">
         <f>IF(ISNUMBER(Mask!N7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="O7" t="str">
         <f>IF(ISNUMBER(Mask!O7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="P7" t="str">
         <f>IF(ISNUMBER(Mask!P7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="Q7" t="str">
         <f>IF(ISNUMBER(Mask!Q7),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="R7" t="str">
         <f>IF(ISNUMBER(Mask!R7),setup!$F$1,"")</f>
@@ -1625,63 +1629,63 @@
       </c>
       <c r="C8" t="str">
         <f>IF(ISNUMBER(Mask!C8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="D8" t="str">
         <f>IF(ISNUMBER(Mask!D8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="E8" t="str">
         <f>IF(ISNUMBER(Mask!E8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="F8" t="str">
         <f>IF(ISNUMBER(Mask!F8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="G8" t="str">
         <f>IF(ISNUMBER(Mask!G8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="H8" t="str">
         <f>IF(ISNUMBER(Mask!H8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="I8" t="str">
         <f>IF(ISNUMBER(Mask!I8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="J8" t="str">
         <f>IF(ISNUMBER(Mask!J8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="K8" t="str">
         <f>IF(ISNUMBER(Mask!K8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="L8" t="str">
         <f>IF(ISNUMBER(Mask!L8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="M8" t="str">
         <f>IF(ISNUMBER(Mask!M8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="N8" t="str">
         <f>IF(ISNUMBER(Mask!N8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="O8" t="str">
         <f>IF(ISNUMBER(Mask!O8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="P8" t="str">
         <f>IF(ISNUMBER(Mask!P8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="Q8" t="str">
         <f>IF(ISNUMBER(Mask!Q8),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="R8" t="str">
         <f>IF(ISNUMBER(Mask!R8),setup!$F$1,"")</f>
@@ -1698,67 +1702,67 @@
       </c>
       <c r="C9" t="str">
         <f>IF(ISNUMBER(Mask!C9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="D9" t="str">
         <f>IF(ISNUMBER(Mask!D9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="E9" t="str">
         <f>IF(ISNUMBER(Mask!E9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="F9" t="str">
         <f>IF(ISNUMBER(Mask!F9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="G9" t="str">
         <f>IF(ISNUMBER(Mask!G9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="H9" t="str">
         <f>IF(ISNUMBER(Mask!H9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="I9" t="str">
         <f>IF(ISNUMBER(Mask!I9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="J9" t="str">
         <f>IF(ISNUMBER(Mask!J9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="K9" t="str">
         <f>IF(ISNUMBER(Mask!K9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="L9" t="str">
         <f>IF(ISNUMBER(Mask!L9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="M9" t="str">
         <f>IF(ISNUMBER(Mask!M9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="N9" t="str">
         <f>IF(ISNUMBER(Mask!N9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="O9" t="str">
         <f>IF(ISNUMBER(Mask!O9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="P9" t="str">
         <f>IF(ISNUMBER(Mask!P9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="Q9" t="str">
         <f>IF(ISNUMBER(Mask!Q9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="R9" t="str">
         <f>IF(ISNUMBER(Mask!R9),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
@@ -1771,67 +1775,67 @@
       </c>
       <c r="C10" t="str">
         <f>IF(ISNUMBER(Mask!C10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="D10" t="str">
         <f>IF(ISNUMBER(Mask!D10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="E10" t="str">
         <f>IF(ISNUMBER(Mask!E10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="F10" t="str">
         <f>IF(ISNUMBER(Mask!F10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="G10" t="str">
         <f>IF(ISNUMBER(Mask!G10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="H10" t="str">
         <f>IF(ISNUMBER(Mask!H10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="I10" t="str">
         <f>IF(ISNUMBER(Mask!I10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="J10" t="str">
         <f>IF(ISNUMBER(Mask!J10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="K10" t="str">
         <f>IF(ISNUMBER(Mask!K10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="L10" t="str">
         <f>IF(ISNUMBER(Mask!L10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="M10" t="str">
         <f>IF(ISNUMBER(Mask!M10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="N10" t="str">
         <f>IF(ISNUMBER(Mask!N10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="O10" t="str">
         <f>IF(ISNUMBER(Mask!O10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="P10" t="str">
         <f>IF(ISNUMBER(Mask!P10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="Q10" t="str">
         <f>IF(ISNUMBER(Mask!Q10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="R10" t="str">
         <f>IF(ISNUMBER(Mask!R10),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
@@ -1844,7 +1848,7 @@
       </c>
       <c r="C11" t="str">
         <f>IF(ISNUMBER(Mask!C11),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="D11" t="str">
         <f>IF(ISNUMBER(Mask!D11),setup!$F$1,"")</f>
@@ -1917,27 +1921,27 @@
       </c>
       <c r="C12" t="str">
         <f>IF(ISNUMBER(Mask!C12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="D12" t="str">
         <f>IF(ISNUMBER(Mask!D12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="E12" t="str">
         <f>IF(ISNUMBER(Mask!E12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="F12" t="str">
         <f>IF(ISNUMBER(Mask!F12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="G12" t="str">
         <f>IF(ISNUMBER(Mask!G12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="H12" t="str">
         <f>IF(ISNUMBER(Mask!H12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="I12" t="str">
         <f>IF(ISNUMBER(Mask!I12),setup!$F$1,"")</f>
@@ -1945,11 +1949,11 @@
       </c>
       <c r="J12" t="str">
         <f>IF(ISNUMBER(Mask!J12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="K12" t="str">
         <f>IF(ISNUMBER(Mask!K12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="L12" t="str">
         <f>IF(ISNUMBER(Mask!L12),setup!$F$1,"")</f>
@@ -1957,27 +1961,27 @@
       </c>
       <c r="M12" t="str">
         <f>IF(ISNUMBER(Mask!M12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="N12" t="str">
         <f>IF(ISNUMBER(Mask!N12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="O12" t="str">
         <f>IF(ISNUMBER(Mask!O12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="P12" t="str">
         <f>IF(ISNUMBER(Mask!P12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="Q12" t="str">
         <f>IF(ISNUMBER(Mask!Q12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="R12" t="str">
         <f>IF(ISNUMBER(Mask!R12),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
@@ -1990,27 +1994,27 @@
       </c>
       <c r="C13" t="str">
         <f>IF(ISNUMBER(Mask!C13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="D13" t="str">
         <f>IF(ISNUMBER(Mask!D13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="E13" t="str">
         <f>IF(ISNUMBER(Mask!E13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="F13" t="str">
         <f>IF(ISNUMBER(Mask!F13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="G13" t="str">
         <f>IF(ISNUMBER(Mask!G13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="H13" t="str">
         <f>IF(ISNUMBER(Mask!H13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="I13" t="str">
         <f>IF(ISNUMBER(Mask!I13),setup!$F$1,"")</f>
@@ -2018,11 +2022,11 @@
       </c>
       <c r="J13" t="str">
         <f>IF(ISNUMBER(Mask!J13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="K13" t="str">
         <f>IF(ISNUMBER(Mask!K13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="L13" t="str">
         <f>IF(ISNUMBER(Mask!L13),setup!$F$1,"")</f>
@@ -2030,27 +2034,27 @@
       </c>
       <c r="M13" t="str">
         <f>IF(ISNUMBER(Mask!M13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="N13" t="str">
         <f>IF(ISNUMBER(Mask!N13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="O13" t="str">
         <f>IF(ISNUMBER(Mask!O13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="P13" t="str">
         <f>IF(ISNUMBER(Mask!P13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="Q13" t="str">
         <f>IF(ISNUMBER(Mask!Q13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="R13" t="str">
         <f>IF(ISNUMBER(Mask!R13),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
@@ -2063,27 +2067,27 @@
       </c>
       <c r="C14" t="str">
         <f>IF(ISNUMBER(Mask!C14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="D14" t="str">
         <f>IF(ISNUMBER(Mask!D14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="E14" t="str">
         <f>IF(ISNUMBER(Mask!E14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="F14" t="str">
         <f>IF(ISNUMBER(Mask!F14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="G14" t="str">
         <f>IF(ISNUMBER(Mask!G14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="H14" t="str">
         <f>IF(ISNUMBER(Mask!H14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="I14" t="str">
         <f>IF(ISNUMBER(Mask!I14),setup!$F$1,"")</f>
@@ -2091,11 +2095,11 @@
       </c>
       <c r="J14" t="str">
         <f>IF(ISNUMBER(Mask!J14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="K14" t="str">
         <f>IF(ISNUMBER(Mask!K14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="L14" t="str">
         <f>IF(ISNUMBER(Mask!L14),setup!$F$1,"")</f>
@@ -2103,27 +2107,27 @@
       </c>
       <c r="M14" t="str">
         <f>IF(ISNUMBER(Mask!M14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="N14" t="str">
         <f>IF(ISNUMBER(Mask!N14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="O14" t="str">
         <f>IF(ISNUMBER(Mask!O14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="P14" t="str">
         <f>IF(ISNUMBER(Mask!P14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="Q14" t="str">
         <f>IF(ISNUMBER(Mask!Q14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="R14" t="str">
         <f>IF(ISNUMBER(Mask!R14),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
@@ -2136,27 +2140,27 @@
       </c>
       <c r="C15" t="str">
         <f>IF(ISNUMBER(Mask!C15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="D15" t="str">
         <f>IF(ISNUMBER(Mask!D15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="E15" t="str">
         <f>IF(ISNUMBER(Mask!E15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="F15" t="str">
         <f>IF(ISNUMBER(Mask!F15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="G15" t="str">
         <f>IF(ISNUMBER(Mask!G15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="H15" t="str">
         <f>IF(ISNUMBER(Mask!H15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="I15" t="str">
         <f>IF(ISNUMBER(Mask!I15),setup!$F$1,"")</f>
@@ -2164,11 +2168,11 @@
       </c>
       <c r="J15" t="str">
         <f>IF(ISNUMBER(Mask!J15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="K15" t="str">
         <f>IF(ISNUMBER(Mask!K15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="L15" t="str">
         <f>IF(ISNUMBER(Mask!L15),setup!$F$1,"")</f>
@@ -2176,27 +2180,27 @@
       </c>
       <c r="M15" t="str">
         <f>IF(ISNUMBER(Mask!M15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="N15" t="str">
         <f>IF(ISNUMBER(Mask!N15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="O15" t="str">
         <f>IF(ISNUMBER(Mask!O15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="P15" t="str">
         <f>IF(ISNUMBER(Mask!P15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="Q15" t="str">
         <f>IF(ISNUMBER(Mask!Q15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="R15" t="str">
         <f>IF(ISNUMBER(Mask!R15),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
@@ -2225,11 +2229,11 @@
       </c>
       <c r="G16" t="str">
         <f>IF(ISNUMBER(Mask!G16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="H16" t="str">
         <f>IF(ISNUMBER(Mask!H16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="I16" t="str">
         <f>IF(ISNUMBER(Mask!I16),setup!$F$1,"")</f>
@@ -2237,11 +2241,11 @@
       </c>
       <c r="J16" t="str">
         <f>IF(ISNUMBER(Mask!J16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="K16" t="str">
         <f>IF(ISNUMBER(Mask!K16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="L16" t="str">
         <f>IF(ISNUMBER(Mask!L16),setup!$F$1,"")</f>
@@ -2249,27 +2253,27 @@
       </c>
       <c r="M16" t="str">
         <f>IF(ISNUMBER(Mask!M16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="N16" t="str">
         <f>IF(ISNUMBER(Mask!N16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="O16" t="str">
         <f>IF(ISNUMBER(Mask!O16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="P16" t="str">
         <f>IF(ISNUMBER(Mask!P16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="Q16" t="str">
         <f>IF(ISNUMBER(Mask!Q16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="R16" t="str">
         <f>IF(ISNUMBER(Mask!R16),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
@@ -2302,7 +2306,7 @@
       </c>
       <c r="H17" t="str">
         <f>IF(ISNUMBER(Mask!H17),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="I17" t="str">
         <f>IF(ISNUMBER(Mask!I17),setup!$F$1,"")</f>
@@ -2310,11 +2314,11 @@
       </c>
       <c r="J17" t="str">
         <f>IF(ISNUMBER(Mask!J17),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="K17" t="str">
         <f>IF(ISNUMBER(Mask!K17),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="L17" t="str">
         <f>IF(ISNUMBER(Mask!L17),setup!$F$1,"")</f>
@@ -2322,7 +2326,7 @@
       </c>
       <c r="M17" t="str">
         <f>IF(ISNUMBER(Mask!M17),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="N17" t="str">
         <f>IF(ISNUMBER(Mask!N17),setup!$F$1,"")</f>
@@ -2383,11 +2387,11 @@
       </c>
       <c r="J18" t="str">
         <f>IF(ISNUMBER(Mask!J18),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="K18" t="str">
         <f>IF(ISNUMBER(Mask!K18),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="L18" t="str">
         <f>IF(ISNUMBER(Mask!L18),setup!$F$1,"")</f>
@@ -2456,11 +2460,11 @@
       </c>
       <c r="J19" t="str">
         <f>IF(ISNUMBER(Mask!J19),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="K19" t="str">
         <f>IF(ISNUMBER(Mask!K19),setup!$F$1,"")</f>
-        <v>138,3,3</v>
+        <v>0,0,0</v>
       </c>
       <c r="L19" t="str">
         <f>IF(ISNUMBER(Mask!L19),setup!$F$1,"")</f>
@@ -2503,11 +2507,1095 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154DB63B-0F2C-489A-9C20-487C41587A71}">
+  <dimension ref="A1:S20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O5" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" t="s">
+        <v>8</v>
+      </c>
+      <c r="P7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>8</v>
+      </c>
+      <c r="R7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" t="s">
+        <v>8</v>
+      </c>
+      <c r="O8" t="s">
+        <v>8</v>
+      </c>
+      <c r="P8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" t="s">
+        <v>8</v>
+      </c>
+      <c r="N9" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" t="s">
+        <v>8</v>
+      </c>
+      <c r="P9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>8</v>
+      </c>
+      <c r="R9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" t="s">
+        <v>3</v>
+      </c>
+      <c r="P10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>3</v>
+      </c>
+      <c r="R10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>1</v>
+      </c>
+      <c r="R11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" t="s">
+        <v>3</v>
+      </c>
+      <c r="O12" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>3</v>
+      </c>
+      <c r="R12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>8</v>
+      </c>
+      <c r="N13" t="s">
+        <v>8</v>
+      </c>
+      <c r="O13" t="s">
+        <v>8</v>
+      </c>
+      <c r="P13" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>8</v>
+      </c>
+      <c r="R13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O14" t="s">
+        <v>8</v>
+      </c>
+      <c r="P14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>8</v>
+      </c>
+      <c r="R14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>3</v>
+      </c>
+      <c r="N15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>8</v>
+      </c>
+      <c r="R15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K16" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" t="s">
+        <v>8</v>
+      </c>
+      <c r="N16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O16" t="s">
+        <v>8</v>
+      </c>
+      <c r="P16" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>8</v>
+      </c>
+      <c r="R16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" t="s">
+        <v>8</v>
+      </c>
+      <c r="N17" t="s">
+        <v>1</v>
+      </c>
+      <c r="O17" t="s">
+        <v>1</v>
+      </c>
+      <c r="P17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18" t="s">
+        <v>8</v>
+      </c>
+      <c r="L18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M18" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18" t="s">
+        <v>1</v>
+      </c>
+      <c r="O18" t="s">
+        <v>1</v>
+      </c>
+      <c r="P18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>8</v>
+      </c>
+      <c r="K19" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" t="s">
+        <v>1</v>
+      </c>
+      <c r="O19" t="s">
+        <v>1</v>
+      </c>
+      <c r="P19" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C3361C-1C15-4A97-8B76-564436F68EDA}">
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I11" sqref="A1:U21"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3772,12 +4860,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF6F8B5-AF9A-4C54-8212-EFBD25DA246B}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
issue in excel where it confuses RGB as date
</commit_message>
<xml_diff>
--- a/blinka/data/grid.xlsx
+++ b/blinka/data/grid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\william.harding\Documents\repos\raspberrypi\blinka\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53345B8-819A-4859-8FA6-EB5BFBFD5AED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D6C326-AC5D-4691-BC5B-25A2A3A77D42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="setup" sheetId="3" r:id="rId1"/>
@@ -18,11 +18,10 @@
     <sheet name="sheetmaker" sheetId="1" r:id="rId3"/>
     <sheet name="pattern 1" sheetId="4" r:id="rId4"/>
     <sheet name="pattern 2" sheetId="5" r:id="rId5"/>
-    <sheet name="pattern 3" sheetId="6" r:id="rId6"/>
-    <sheet name="pattern 4" sheetId="7" r:id="rId7"/>
-    <sheet name="pattern 5" sheetId="8" r:id="rId8"/>
-    <sheet name="pattern 6" sheetId="9" r:id="rId9"/>
-    <sheet name="pattern 7" sheetId="10" r:id="rId10"/>
+    <sheet name="pattern 4" sheetId="7" r:id="rId6"/>
+    <sheet name="pattern 5" sheetId="8" r:id="rId7"/>
+    <sheet name="pattern 6" sheetId="9" r:id="rId8"/>
+    <sheet name="pattern 7" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1964" uniqueCount="7">
   <si>
     <t>default color</t>
   </si>
@@ -99,9 +98,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,1090 +439,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2BC27F6-5F3F-4BE2-9D95-BFC21BF9813F}">
-  <dimension ref="A1:S20"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-      <c r="N1">
-        <v>13</v>
-      </c>
-      <c r="O1">
-        <v>14</v>
-      </c>
-      <c r="P1">
-        <v>15</v>
-      </c>
-      <c r="Q1">
-        <v>16</v>
-      </c>
-      <c r="R1">
-        <v>17</v>
-      </c>
-      <c r="S1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" t="s">
-        <v>1</v>
-      </c>
-      <c r="P3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>1</v>
-      </c>
-      <c r="R3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" t="s">
-        <v>6</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P4" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>1</v>
-      </c>
-      <c r="R4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" t="s">
-        <v>6</v>
-      </c>
-      <c r="N5" t="s">
-        <v>6</v>
-      </c>
-      <c r="O5" t="s">
-        <v>6</v>
-      </c>
-      <c r="P5" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>1</v>
-      </c>
-      <c r="R5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6" t="s">
-        <v>6</v>
-      </c>
-      <c r="N6" t="s">
-        <v>6</v>
-      </c>
-      <c r="O6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P6" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>1</v>
-      </c>
-      <c r="R6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" t="s">
-        <v>6</v>
-      </c>
-      <c r="M7" t="s">
-        <v>6</v>
-      </c>
-      <c r="N7" t="s">
-        <v>6</v>
-      </c>
-      <c r="O7" t="s">
-        <v>6</v>
-      </c>
-      <c r="P7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>6</v>
-      </c>
-      <c r="R7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M8" t="s">
-        <v>6</v>
-      </c>
-      <c r="N8" t="s">
-        <v>6</v>
-      </c>
-      <c r="O8" t="s">
-        <v>6</v>
-      </c>
-      <c r="P8" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>6</v>
-      </c>
-      <c r="R8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L9" t="s">
-        <v>6</v>
-      </c>
-      <c r="M9" t="s">
-        <v>6</v>
-      </c>
-      <c r="N9" t="s">
-        <v>6</v>
-      </c>
-      <c r="O9" t="s">
-        <v>6</v>
-      </c>
-      <c r="P9" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>6</v>
-      </c>
-      <c r="R9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>3</v>
-      </c>
-      <c r="H10" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K10" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" t="s">
-        <v>6</v>
-      </c>
-      <c r="M10" t="s">
-        <v>3</v>
-      </c>
-      <c r="N10" t="s">
-        <v>3</v>
-      </c>
-      <c r="O10" t="s">
-        <v>3</v>
-      </c>
-      <c r="P10" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>3</v>
-      </c>
-      <c r="R10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L11" t="s">
-        <v>1</v>
-      </c>
-      <c r="M11" t="s">
-        <v>1</v>
-      </c>
-      <c r="N11" t="s">
-        <v>1</v>
-      </c>
-      <c r="O11" t="s">
-        <v>1</v>
-      </c>
-      <c r="P11" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>1</v>
-      </c>
-      <c r="R11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>6</v>
-      </c>
-      <c r="K12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L12" t="s">
-        <v>1</v>
-      </c>
-      <c r="M12" t="s">
-        <v>3</v>
-      </c>
-      <c r="N12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O12" t="s">
-        <v>3</v>
-      </c>
-      <c r="P12" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>3</v>
-      </c>
-      <c r="R12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" t="s">
-        <v>1</v>
-      </c>
-      <c r="J13" t="s">
-        <v>6</v>
-      </c>
-      <c r="K13" t="s">
-        <v>6</v>
-      </c>
-      <c r="L13" t="s">
-        <v>1</v>
-      </c>
-      <c r="M13" t="s">
-        <v>6</v>
-      </c>
-      <c r="N13" t="s">
-        <v>6</v>
-      </c>
-      <c r="O13" t="s">
-        <v>6</v>
-      </c>
-      <c r="P13" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>6</v>
-      </c>
-      <c r="R13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" t="s">
-        <v>3</v>
-      </c>
-      <c r="I14" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" t="s">
-        <v>6</v>
-      </c>
-      <c r="K14" t="s">
-        <v>6</v>
-      </c>
-      <c r="L14" t="s">
-        <v>1</v>
-      </c>
-      <c r="M14" t="s">
-        <v>3</v>
-      </c>
-      <c r="N14" t="s">
-        <v>3</v>
-      </c>
-      <c r="O14" t="s">
-        <v>6</v>
-      </c>
-      <c r="P14" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>6</v>
-      </c>
-      <c r="R14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H15" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" t="s">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
-        <v>6</v>
-      </c>
-      <c r="K15" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M15" t="s">
-        <v>6</v>
-      </c>
-      <c r="N15" t="s">
-        <v>6</v>
-      </c>
-      <c r="O15" t="s">
-        <v>3</v>
-      </c>
-      <c r="P15" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>6</v>
-      </c>
-      <c r="R15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" t="s">
-        <v>3</v>
-      </c>
-      <c r="L16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M16" t="s">
-        <v>3</v>
-      </c>
-      <c r="N16" t="s">
-        <v>3</v>
-      </c>
-      <c r="O16" t="s">
-        <v>6</v>
-      </c>
-      <c r="P16" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>6</v>
-      </c>
-      <c r="R16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L17" t="s">
-        <v>1</v>
-      </c>
-      <c r="M17" t="s">
-        <v>6</v>
-      </c>
-      <c r="N17" t="s">
-        <v>1</v>
-      </c>
-      <c r="O17" t="s">
-        <v>1</v>
-      </c>
-      <c r="P17" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>1</v>
-      </c>
-      <c r="R17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" t="s">
-        <v>3</v>
-      </c>
-      <c r="K18" t="s">
-        <v>3</v>
-      </c>
-      <c r="L18" t="s">
-        <v>1</v>
-      </c>
-      <c r="M18" t="s">
-        <v>1</v>
-      </c>
-      <c r="N18" t="s">
-        <v>1</v>
-      </c>
-      <c r="O18" t="s">
-        <v>1</v>
-      </c>
-      <c r="P18" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>1</v>
-      </c>
-      <c r="R18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" t="s">
-        <v>1</v>
-      </c>
-      <c r="I19" t="s">
-        <v>1</v>
-      </c>
-      <c r="J19" t="s">
-        <v>6</v>
-      </c>
-      <c r="K19" t="s">
-        <v>6</v>
-      </c>
-      <c r="L19" t="s">
-        <v>1</v>
-      </c>
-      <c r="M19" t="s">
-        <v>1</v>
-      </c>
-      <c r="N19" t="s">
-        <v>1</v>
-      </c>
-      <c r="O19" t="s">
-        <v>1</v>
-      </c>
-      <c r="P19" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>1</v>
-      </c>
-      <c r="R19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7823F826-DB8C-4CD7-AE29-877D52C9DD1E}">
   <dimension ref="A1:S20"/>
@@ -2199,7 +1113,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView zoomScale="61" workbookViewId="0">
-      <selection activeCell="E16" sqref="A1:S20"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3593,8 +2507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C3361C-1C15-4A97-8B76-564436F68EDA}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="A1:U21"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4864,7 +3778,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="A1:U21"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6129,1285 +5043,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154DB63B-0F2C-489A-9C20-487C41587A71}">
-  <dimension ref="A1:U21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:P1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="10.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-      <c r="N1">
-        <v>13</v>
-      </c>
-      <c r="O1">
-        <v>14</v>
-      </c>
-      <c r="P1">
-        <v>15</v>
-      </c>
-      <c r="Q1">
-        <v>16</v>
-      </c>
-      <c r="R1">
-        <v>17</v>
-      </c>
-      <c r="S1">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>1</v>
-      </c>
-      <c r="U1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" t="s">
-        <v>1</v>
-      </c>
-      <c r="U2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" t="s">
-        <v>1</v>
-      </c>
-      <c r="P3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>1</v>
-      </c>
-      <c r="R3" t="s">
-        <v>1</v>
-      </c>
-      <c r="T3" t="s">
-        <v>1</v>
-      </c>
-      <c r="U3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" t="s">
-        <v>6</v>
-      </c>
-      <c r="N4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P4" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>1</v>
-      </c>
-      <c r="R4" t="s">
-        <v>1</v>
-      </c>
-      <c r="T4" t="s">
-        <v>1</v>
-      </c>
-      <c r="U4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" t="s">
-        <v>6</v>
-      </c>
-      <c r="N5" t="s">
-        <v>6</v>
-      </c>
-      <c r="O5" t="s">
-        <v>6</v>
-      </c>
-      <c r="P5" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>1</v>
-      </c>
-      <c r="R5" t="s">
-        <v>1</v>
-      </c>
-      <c r="T5" t="s">
-        <v>1</v>
-      </c>
-      <c r="U5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6" t="s">
-        <v>6</v>
-      </c>
-      <c r="N6" t="s">
-        <v>6</v>
-      </c>
-      <c r="O6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P6" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>1</v>
-      </c>
-      <c r="R6" t="s">
-        <v>1</v>
-      </c>
-      <c r="T6" t="s">
-        <v>1</v>
-      </c>
-      <c r="U6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" t="s">
-        <v>6</v>
-      </c>
-      <c r="M7" t="s">
-        <v>6</v>
-      </c>
-      <c r="N7" t="s">
-        <v>6</v>
-      </c>
-      <c r="O7" t="s">
-        <v>6</v>
-      </c>
-      <c r="P7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>6</v>
-      </c>
-      <c r="R7" t="s">
-        <v>1</v>
-      </c>
-      <c r="T7" t="s">
-        <v>1</v>
-      </c>
-      <c r="U7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M8" t="s">
-        <v>6</v>
-      </c>
-      <c r="N8" t="s">
-        <v>6</v>
-      </c>
-      <c r="O8" t="s">
-        <v>6</v>
-      </c>
-      <c r="P8" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>6</v>
-      </c>
-      <c r="R8" t="s">
-        <v>1</v>
-      </c>
-      <c r="T8" t="s">
-        <v>1</v>
-      </c>
-      <c r="U8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L9" t="s">
-        <v>6</v>
-      </c>
-      <c r="M9" t="s">
-        <v>6</v>
-      </c>
-      <c r="N9" t="s">
-        <v>6</v>
-      </c>
-      <c r="O9" t="s">
-        <v>6</v>
-      </c>
-      <c r="P9" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>6</v>
-      </c>
-      <c r="R9" t="s">
-        <v>6</v>
-      </c>
-      <c r="T9" t="s">
-        <v>1</v>
-      </c>
-      <c r="U9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="E10" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="F10" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="G10" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="H10" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K10" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" t="s">
-        <v>6</v>
-      </c>
-      <c r="M10" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="N10" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="O10" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="P10" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>6</v>
-      </c>
-      <c r="R10" t="s">
-        <v>6</v>
-      </c>
-      <c r="T10" t="s">
-        <v>1</v>
-      </c>
-      <c r="U10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
-        <v>1</v>
-      </c>
-      <c r="L11" t="s">
-        <v>1</v>
-      </c>
-      <c r="M11" t="s">
-        <v>1</v>
-      </c>
-      <c r="N11" t="s">
-        <v>1</v>
-      </c>
-      <c r="O11" t="s">
-        <v>1</v>
-      </c>
-      <c r="P11" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>1</v>
-      </c>
-      <c r="R11" t="s">
-        <v>1</v>
-      </c>
-      <c r="T11" t="s">
-        <v>1</v>
-      </c>
-      <c r="U11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="E12" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="F12" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="G12" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="H12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>6</v>
-      </c>
-      <c r="K12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L12" t="s">
-        <v>1</v>
-      </c>
-      <c r="M12" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="N12" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="O12" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="P12" s="1">
-        <v>197205216</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>6</v>
-      </c>
-      <c r="R12" t="s">
-        <v>6</v>
-      </c>
-      <c r="T12" t="s">
-        <v>1</v>
-      </c>
-      <c r="U12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" t="s">
-        <v>1</v>
-      </c>
-      <c r="J13" t="s">
-        <v>6</v>
-      </c>
-      <c r="K13" t="s">
-        <v>6</v>
-      </c>
-      <c r="L13" t="s">
-        <v>1</v>
-      </c>
-      <c r="M13" t="s">
-        <v>6</v>
-      </c>
-      <c r="N13" t="s">
-        <v>6</v>
-      </c>
-      <c r="O13" t="s">
-        <v>6</v>
-      </c>
-      <c r="P13" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>6</v>
-      </c>
-      <c r="R13" t="s">
-        <v>6</v>
-      </c>
-      <c r="T13" t="s">
-        <v>1</v>
-      </c>
-      <c r="U13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" t="s">
-        <v>6</v>
-      </c>
-      <c r="K14" t="s">
-        <v>6</v>
-      </c>
-      <c r="L14" t="s">
-        <v>1</v>
-      </c>
-      <c r="M14" t="s">
-        <v>6</v>
-      </c>
-      <c r="N14" t="s">
-        <v>6</v>
-      </c>
-      <c r="O14" t="s">
-        <v>6</v>
-      </c>
-      <c r="P14" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>6</v>
-      </c>
-      <c r="R14" t="s">
-        <v>6</v>
-      </c>
-      <c r="T14" t="s">
-        <v>1</v>
-      </c>
-      <c r="U14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" t="s">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
-        <v>6</v>
-      </c>
-      <c r="K15" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" t="s">
-        <v>1</v>
-      </c>
-      <c r="M15" t="s">
-        <v>6</v>
-      </c>
-      <c r="N15" t="s">
-        <v>6</v>
-      </c>
-      <c r="O15" t="s">
-        <v>6</v>
-      </c>
-      <c r="P15" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>6</v>
-      </c>
-      <c r="R15" t="s">
-        <v>6</v>
-      </c>
-      <c r="T15" t="s">
-        <v>1</v>
-      </c>
-      <c r="U15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I16" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" t="s">
-        <v>6</v>
-      </c>
-      <c r="K16" t="s">
-        <v>6</v>
-      </c>
-      <c r="L16" t="s">
-        <v>1</v>
-      </c>
-      <c r="M16" t="s">
-        <v>6</v>
-      </c>
-      <c r="N16" t="s">
-        <v>6</v>
-      </c>
-      <c r="O16" t="s">
-        <v>6</v>
-      </c>
-      <c r="P16" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>6</v>
-      </c>
-      <c r="R16" t="s">
-        <v>6</v>
-      </c>
-      <c r="T16" t="s">
-        <v>1</v>
-      </c>
-      <c r="U16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L17" t="s">
-        <v>1</v>
-      </c>
-      <c r="M17" t="s">
-        <v>6</v>
-      </c>
-      <c r="N17" t="s">
-        <v>1</v>
-      </c>
-      <c r="O17" t="s">
-        <v>1</v>
-      </c>
-      <c r="P17" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>1</v>
-      </c>
-      <c r="R17" t="s">
-        <v>1</v>
-      </c>
-      <c r="T17" t="s">
-        <v>1</v>
-      </c>
-      <c r="U17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" t="s">
-        <v>6</v>
-      </c>
-      <c r="K18" t="s">
-        <v>6</v>
-      </c>
-      <c r="L18" t="s">
-        <v>1</v>
-      </c>
-      <c r="M18" t="s">
-        <v>1</v>
-      </c>
-      <c r="N18" t="s">
-        <v>1</v>
-      </c>
-      <c r="O18" t="s">
-        <v>1</v>
-      </c>
-      <c r="P18" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>1</v>
-      </c>
-      <c r="R18" t="s">
-        <v>1</v>
-      </c>
-      <c r="T18" t="s">
-        <v>1</v>
-      </c>
-      <c r="U18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" t="s">
-        <v>1</v>
-      </c>
-      <c r="I19" t="s">
-        <v>1</v>
-      </c>
-      <c r="J19" t="s">
-        <v>6</v>
-      </c>
-      <c r="K19" t="s">
-        <v>6</v>
-      </c>
-      <c r="L19" t="s">
-        <v>1</v>
-      </c>
-      <c r="M19" t="s">
-        <v>1</v>
-      </c>
-      <c r="N19" t="s">
-        <v>1</v>
-      </c>
-      <c r="O19" t="s">
-        <v>1</v>
-      </c>
-      <c r="P19" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>1</v>
-      </c>
-      <c r="R19" t="s">
-        <v>1</v>
-      </c>
-      <c r="T19" t="s">
-        <v>1</v>
-      </c>
-      <c r="U19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="T20" t="s">
-        <v>1</v>
-      </c>
-      <c r="U20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>1</v>
-      </c>
-      <c r="H21" t="s">
-        <v>1</v>
-      </c>
-      <c r="I21" t="s">
-        <v>1</v>
-      </c>
-      <c r="J21" t="s">
-        <v>1</v>
-      </c>
-      <c r="K21" t="s">
-        <v>1</v>
-      </c>
-      <c r="L21" t="s">
-        <v>1</v>
-      </c>
-      <c r="M21" t="s">
-        <v>1</v>
-      </c>
-      <c r="N21" t="s">
-        <v>1</v>
-      </c>
-      <c r="O21" t="s">
-        <v>1</v>
-      </c>
-      <c r="P21" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>1</v>
-      </c>
-      <c r="R21" t="s">
-        <v>1</v>
-      </c>
-      <c r="S21" t="s">
-        <v>1</v>
-      </c>
-      <c r="T21" t="s">
-        <v>1</v>
-      </c>
-      <c r="U21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558688A1-2D04-476E-9547-CEAEC11E5A7D}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
@@ -8487,7 +6126,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D501871-2A8F-43B2-8FDF-99770314150F}">
   <dimension ref="A1:S20"/>
   <sheetViews>
@@ -9571,7 +7210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2FDCE88-BFB6-433D-AA87-37E2767C94B9}">
   <dimension ref="A1:S20"/>
   <sheetViews>
@@ -10653,4 +8292,1088 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2BC27F6-5F3F-4BE2-9D95-BFC21BF9813F}">
+  <dimension ref="A1:S20"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>6</v>
+      </c>
+      <c r="R8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" t="s">
+        <v>3</v>
+      </c>
+      <c r="P10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>3</v>
+      </c>
+      <c r="R10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>1</v>
+      </c>
+      <c r="R11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" t="s">
+        <v>1</v>
+      </c>
+      <c r="M12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" t="s">
+        <v>3</v>
+      </c>
+      <c r="O12" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>3</v>
+      </c>
+      <c r="R12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>6</v>
+      </c>
+      <c r="N13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O13" t="s">
+        <v>6</v>
+      </c>
+      <c r="P13" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>6</v>
+      </c>
+      <c r="R13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" t="s">
+        <v>6</v>
+      </c>
+      <c r="L14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" t="s">
+        <v>6</v>
+      </c>
+      <c r="P14" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>6</v>
+      </c>
+      <c r="R14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" t="s">
+        <v>6</v>
+      </c>
+      <c r="O15" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>6</v>
+      </c>
+      <c r="R15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" t="s">
+        <v>3</v>
+      </c>
+      <c r="L16" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" t="s">
+        <v>6</v>
+      </c>
+      <c r="P16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>6</v>
+      </c>
+      <c r="R16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" t="s">
+        <v>6</v>
+      </c>
+      <c r="N17" t="s">
+        <v>1</v>
+      </c>
+      <c r="O17" t="s">
+        <v>1</v>
+      </c>
+      <c r="P17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" t="s">
+        <v>3</v>
+      </c>
+      <c r="L18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M18" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18" t="s">
+        <v>1</v>
+      </c>
+      <c r="O18" t="s">
+        <v>1</v>
+      </c>
+      <c r="P18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" t="s">
+        <v>1</v>
+      </c>
+      <c r="M19" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" t="s">
+        <v>1</v>
+      </c>
+      <c r="O19" t="s">
+        <v>1</v>
+      </c>
+      <c r="P19" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>